<commit_message>
TS Jatai working files 30/05/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Vowel Elongation" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Avagraha" sheetId="7" r:id="rId7"/>
     <sheet name="Special Anuswaram" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511" iterate="1"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1888" uniqueCount="1190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1964" uniqueCount="1191">
   <si>
     <t xml:space="preserve">PrAtiSakyam Rules </t>
   </si>
@@ -3763,6 +3763,9 @@
   </si>
   <si>
     <t>Y/N</t>
+  </si>
+  <si>
+    <t>Raja</t>
   </si>
 </sst>
 </file>
@@ -3891,7 +3894,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3940,6 +3943,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -3968,7 +3977,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4046,6 +4055,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9848,13 +9858,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J45"/>
+  <dimension ref="A2:K45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomRight" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9868,17 +9878,17 @@
     <col min="7" max="7" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="C2" s="1" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C3" s="8" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>340</v>
       </c>
@@ -9896,7 +9906,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5.4</v>
       </c>
@@ -9912,8 +9922,11 @@
       <c r="H6" s="4" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K6" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5.4</v>
       </c>
@@ -9929,8 +9942,11 @@
       <c r="H7" s="4" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K7" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>5.5</v>
       </c>
@@ -9946,8 +9962,11 @@
       <c r="H8" s="4" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K8" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>5.6</v>
       </c>
@@ -9963,8 +9982,11 @@
       <c r="H9" s="4" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K9" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>5.7</v>
       </c>
@@ -9978,7 +10000,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>5.8</v>
       </c>
@@ -9994,8 +10016,11 @@
       <c r="H11" s="4" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K11" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>5.9</v>
       </c>
@@ -10012,7 +10037,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="27">
         <v>5.0999999999999996</v>
       </c>
@@ -10035,7 +10060,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="27">
         <v>5.0999999999999996</v>
       </c>
@@ -10058,7 +10083,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="27">
         <v>5.0999999999999996</v>
       </c>
@@ -10081,7 +10106,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>5.1100000000000003</v>
       </c>
@@ -10089,7 +10114,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>5.12</v>
       </c>
@@ -10102,8 +10127,11 @@
       <c r="F17" s="4" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K17" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>5.13</v>
       </c>
@@ -10122,8 +10150,11 @@
       <c r="I18" s="4" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K18" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>5.13</v>
       </c>
@@ -10142,8 +10173,11 @@
       <c r="I19" s="4" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K19" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>5.14</v>
       </c>
@@ -10162,8 +10196,11 @@
       <c r="I20" s="4" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K20" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>5.15</v>
       </c>
@@ -10177,7 +10214,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>5.15</v>
       </c>
@@ -10191,7 +10228,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>5.15</v>
       </c>
@@ -10205,7 +10242,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>5.16</v>
       </c>
@@ -10216,7 +10253,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>5.17</v>
       </c>
@@ -10226,8 +10263,11 @@
       <c r="F25" s="4" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K25" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>5.17</v>
       </c>
@@ -10237,8 +10277,11 @@
       <c r="F26" s="4" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K26" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>5.17</v>
       </c>
@@ -10248,8 +10291,11 @@
       <c r="F27" s="4" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K27" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>5.17</v>
       </c>
@@ -10259,8 +10305,11 @@
       <c r="F28" s="4" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K28" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>5.17</v>
       </c>
@@ -10270,8 +10319,11 @@
       <c r="F29" s="4" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K29" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>5.18</v>
       </c>
@@ -10282,7 +10334,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>5.19</v>
       </c>
@@ -10293,7 +10345,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A32" s="27">
         <v>5.2</v>
       </c>
@@ -10443,11 +10495,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="D96" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomRight" activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10462,13 +10514,13 @@
     <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
         <v>400</v>
       </c>
@@ -10476,7 +10528,7 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
@@ -10494,7 +10546,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>6.2</v>
       </c>
@@ -10510,8 +10562,11 @@
       <c r="I6" s="4" t="s">
         <v>1023</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K6" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C7" s="4" t="s">
         <v>403</v>
       </c>
@@ -10524,8 +10579,11 @@
       <c r="I7" s="4" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K7" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C8" s="4" t="s">
         <v>404</v>
       </c>
@@ -10538,8 +10596,11 @@
       <c r="I8" s="4" t="s">
         <v>1020</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K8" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C9" s="4" t="s">
         <v>405</v>
       </c>
@@ -10552,8 +10613,11 @@
       <c r="I9" s="4" t="s">
         <v>1025</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K9" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C10" s="4" t="s">
         <v>606</v>
       </c>
@@ -10563,8 +10627,11 @@
       <c r="F10" s="4" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K10" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C11" s="4" t="s">
         <v>406</v>
       </c>
@@ -10574,8 +10641,11 @@
       <c r="F11" s="4" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K11" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C12" s="4" t="s">
         <v>407</v>
       </c>
@@ -10585,8 +10655,11 @@
       <c r="F12" s="4" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K12" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C13" s="4" t="s">
         <v>408</v>
       </c>
@@ -10596,8 +10669,11 @@
       <c r="F13" s="4" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K13" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C14" s="4" t="s">
         <v>1026</v>
       </c>
@@ -10610,8 +10686,11 @@
       <c r="I14" s="4" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K14" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C15" s="4" t="s">
         <v>409</v>
       </c>
@@ -10624,8 +10703,11 @@
       <c r="I15" s="4" t="s">
         <v>1028</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K15" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C16" s="4" t="s">
         <v>410</v>
       </c>
@@ -10638,14 +10720,17 @@
       <c r="I16" s="4" t="s">
         <v>987</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K16" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C17" s="4" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>6.3</v>
       </c>
@@ -10655,17 +10740,19 @@
       <c r="I19" s="4" t="s">
         <v>1029</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C20" s="4" t="s">
         <v>415</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>1030</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>6.4</v>
       </c>
@@ -10673,8 +10760,8 @@
         <v>975</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>6.5</v>
       </c>
@@ -10690,8 +10777,9 @@
       <c r="F24" s="4" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>6.5</v>
       </c>
@@ -10707,8 +10795,9 @@
       <c r="F25" s="4" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K25" s="6"/>
+    </row>
+    <row r="26" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>6.5</v>
       </c>
@@ -10721,8 +10810,11 @@
       <c r="F26" s="4" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K26" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>6.5</v>
       </c>
@@ -10735,8 +10827,11 @@
       <c r="F27" s="4" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K27" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>6.5</v>
       </c>
@@ -10749,8 +10844,11 @@
       <c r="F28" s="4" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K28" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>6.5</v>
       </c>
@@ -10763,8 +10861,11 @@
       <c r="F29" s="4" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K29" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>6.5</v>
       </c>
@@ -10777,8 +10878,11 @@
       <c r="F30" s="4" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K30" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>6.5</v>
       </c>
@@ -10791,8 +10895,11 @@
       <c r="F31" s="4" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K31" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>6.5</v>
       </c>
@@ -10805,8 +10912,11 @@
       <c r="F32" s="4" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K32" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>6.5</v>
       </c>
@@ -10819,8 +10929,11 @@
       <c r="F33" s="4" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K33" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>6.5</v>
       </c>
@@ -10833,8 +10946,11 @@
       <c r="F34" s="4" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K34" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>6.5</v>
       </c>
@@ -10847,8 +10963,11 @@
       <c r="F35" s="4" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K35" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>6.5</v>
       </c>
@@ -10861,8 +10980,11 @@
       <c r="F36" s="4" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K36" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>6.5</v>
       </c>
@@ -10875,9 +10997,12 @@
       <c r="F37" s="4" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K37" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>6.13</v>
       </c>
@@ -10885,58 +11010,67 @@
         <v>457</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C40" s="4" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C41" s="4" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C42" s="4" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C43" s="4" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C44" s="4" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C45" s="4" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C46" s="4" t="s">
         <v>464</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H46" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C47" s="4" t="s">
         <v>464</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H47" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C48" s="4" t="s">
         <v>464</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>467</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>1190</v>
       </c>
     </row>
     <row r="49" spans="1:3" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -11495,10 +11629,10 @@
   <dimension ref="A3:L294"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D135" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D122" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="M68" sqref="M68"/>
+      <selection pane="bottomRight" activeCell="K139" sqref="K139:K145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11512,10 +11646,10 @@
     <col min="8" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="F3" s="8"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
@@ -11533,8 +11667,8 @@
         <v>412</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>7.2</v>
       </c>
@@ -11547,8 +11681,11 @@
       <c r="F7" s="4" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K7" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C8" s="4" t="s">
         <v>910</v>
       </c>
@@ -11558,8 +11695,11 @@
       <c r="F8" s="4" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K8" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C9" s="4" t="s">
         <v>483</v>
       </c>
@@ -11572,8 +11712,11 @@
       <c r="G9" s="4" t="s">
         <v>950</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K9" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C10" s="4" t="s">
         <v>484</v>
       </c>
@@ -11586,8 +11729,11 @@
       <c r="G10" s="4" t="s">
         <v>951</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K10" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C11" s="4" t="s">
         <v>485</v>
       </c>
@@ -11600,8 +11746,11 @@
       <c r="G11" s="4" t="s">
         <v>952</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K11" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C12" s="4" t="s">
         <v>486</v>
       </c>
@@ -11620,8 +11769,11 @@
       <c r="I12" s="4" t="s">
         <v>953</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K12" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C13" s="4" t="s">
         <v>487</v>
       </c>
@@ -11634,8 +11786,11 @@
       <c r="G13" s="4" t="s">
         <v>956</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K13" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C14" s="4" t="s">
         <v>488</v>
       </c>
@@ -11645,8 +11800,11 @@
       <c r="F14" s="4" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K14" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C15" s="4" t="s">
         <v>489</v>
       </c>
@@ -11659,8 +11817,11 @@
       <c r="G15" s="4" t="s">
         <v>957</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K15" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C16" s="4" t="s">
         <v>490</v>
       </c>
@@ -11670,8 +11831,11 @@
       <c r="F16" s="4" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K16" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C17" s="4" t="s">
         <v>419</v>
       </c>
@@ -11681,9 +11845,12 @@
       <c r="F17" s="4" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K17" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>7.3</v>
       </c>
@@ -11691,7 +11858,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C20" s="4" t="s">
         <v>492</v>
       </c>
@@ -11699,8 +11866,8 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>7.4</v>
       </c>
@@ -11710,32 +11877,44 @@
       <c r="F22" s="4" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K22" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C23" s="4" t="s">
         <v>493</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K23" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C24" s="4" t="s">
         <v>71</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K24" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C25" s="4" t="s">
         <v>281</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K25" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>7.5</v>
       </c>
@@ -11743,8 +11922,8 @@
         <v>494</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>7.6</v>
       </c>
@@ -11757,8 +11936,9 @@
       <c r="H28" s="4" t="s">
         <v>1009</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K28" s="51"/>
+    </row>
+    <row r="29" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C29" s="4" t="s">
         <v>496</v>
       </c>
@@ -11774,40 +11954,46 @@
       <c r="J29" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K29" s="51"/>
+    </row>
+    <row r="30" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C30" s="4" t="s">
         <v>497</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>1012</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K30" s="51"/>
+    </row>
+    <row r="31" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C31" s="4" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K31" s="51"/>
+    </row>
+    <row r="32" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C32" s="4" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K32" s="51"/>
+    </row>
+    <row r="33" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C33" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K33" s="51"/>
+    </row>
+    <row r="34" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>7.7</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K34" s="51"/>
+    </row>
+    <row r="35" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>7.8</v>
       </c>
@@ -11823,8 +12009,11 @@
       <c r="G36" s="4" t="s">
         <v>1002</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K36" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C37" s="4" t="s">
         <v>501</v>
       </c>
@@ -11837,9 +12026,12 @@
       <c r="G37" s="4" t="s">
         <v>1003</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K37" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>7.9</v>
       </c>
@@ -11855,8 +12047,11 @@
       <c r="G39" s="4" t="s">
         <v>1003</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K39" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C40" s="4" t="s">
         <v>505</v>
       </c>
@@ -11869,42 +12064,63 @@
       <c r="G40" s="4" t="s">
         <v>1003</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K40" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>507</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K42" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C43" s="4" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K43" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C44" s="4" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K44" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C45" s="4" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K45" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C46" s="4" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K46" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C47" s="4" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+      <c r="K47" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
     <row r="49" spans="1:6" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>7.11</v>
@@ -12303,6 +12519,9 @@
       <c r="C94" s="4" t="s">
         <v>630</v>
       </c>
+      <c r="E94" s="4" t="s">
+        <v>629</v>
+      </c>
       <c r="F94" s="4" t="s">
         <v>841</v>
       </c>
@@ -12311,6 +12530,9 @@
       <c r="C95" s="4" t="s">
         <v>631</v>
       </c>
+      <c r="E95" s="4" t="s">
+        <v>629</v>
+      </c>
       <c r="F95" s="4" t="s">
         <v>841</v>
       </c>
@@ -12319,6 +12541,9 @@
       <c r="C96" s="4" t="s">
         <v>632</v>
       </c>
+      <c r="E96" s="4" t="s">
+        <v>629</v>
+      </c>
       <c r="F96" s="4" t="s">
         <v>841</v>
       </c>
@@ -12327,6 +12552,9 @@
       <c r="C97" s="4" t="s">
         <v>633</v>
       </c>
+      <c r="E97" s="4" t="s">
+        <v>629</v>
+      </c>
       <c r="F97" s="4" t="s">
         <v>841</v>
       </c>
@@ -12335,6 +12563,9 @@
       <c r="C98" s="4" t="s">
         <v>634</v>
       </c>
+      <c r="E98" s="4" t="s">
+        <v>629</v>
+      </c>
       <c r="F98" s="4" t="s">
         <v>841</v>
       </c>
@@ -12343,6 +12574,9 @@
       <c r="C99" s="4" t="s">
         <v>635</v>
       </c>
+      <c r="E99" s="4" t="s">
+        <v>629</v>
+      </c>
       <c r="F99" s="4" t="s">
         <v>841</v>
       </c>
@@ -12351,6 +12585,9 @@
       <c r="C100" s="4" t="s">
         <v>636</v>
       </c>
+      <c r="E100" s="4" t="s">
+        <v>629</v>
+      </c>
       <c r="F100" s="4" t="s">
         <v>841</v>
       </c>
@@ -12359,6 +12596,9 @@
       <c r="C101" s="4" t="s">
         <v>637</v>
       </c>
+      <c r="E101" s="4" t="s">
+        <v>629</v>
+      </c>
       <c r="F101" s="4" t="s">
         <v>841</v>
       </c>
@@ -12367,6 +12607,9 @@
       <c r="C102" s="4" t="s">
         <v>638</v>
       </c>
+      <c r="E102" s="4" t="s">
+        <v>629</v>
+      </c>
       <c r="F102" s="4" t="s">
         <v>841</v>
       </c>
@@ -12375,6 +12618,9 @@
       <c r="C103" s="4" t="s">
         <v>1141</v>
       </c>
+      <c r="E103" s="4" t="s">
+        <v>629</v>
+      </c>
       <c r="F103" s="4" t="s">
         <v>841</v>
       </c>
@@ -12382,6 +12628,9 @@
     <row r="104" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C104" s="4" t="s">
         <v>639</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>629</v>
       </c>
       <c r="F104" s="4" t="s">
         <v>841</v>
@@ -12727,7 +12976,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="129" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C129" s="4" t="s">
         <v>660</v>
       </c>
@@ -12738,7 +12987,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="130" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C130" s="4" t="s">
         <v>661</v>
       </c>
@@ -12749,8 +12998,8 @@
         <v>654</v>
       </c>
     </row>
-    <row r="131" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="132" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="132" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A132" s="4">
         <v>9.24</v>
       </c>
@@ -12764,7 +13013,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="133" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C133" s="4" t="s">
         <v>662</v>
       </c>
@@ -12775,8 +13024,8 @@
         <v>654</v>
       </c>
     </row>
-    <row r="134" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="135" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="135" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A135" s="4">
         <v>13.6</v>
       </c>
@@ -12790,7 +13039,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="136" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E136" s="4" t="s">
         <v>882</v>
       </c>
@@ -12798,7 +13047,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="137" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E137" s="4" t="s">
         <v>367</v>
       </c>
@@ -12806,7 +13055,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="138" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E138" s="4" t="s">
         <v>360</v>
       </c>
@@ -12814,7 +13063,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="139" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A139" s="4">
         <v>13.5</v>
       </c>
@@ -12824,52 +13073,59 @@
       <c r="G139" s="4" t="s">
         <v>884</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K139" s="51"/>
+    </row>
+    <row r="140" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G140" s="4" t="s">
         <v>885</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K140" s="51"/>
+    </row>
+    <row r="141" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G141" s="4" t="s">
         <v>886</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K141" s="51"/>
+    </row>
+    <row r="142" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G142" s="4" t="s">
         <v>887</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K142" s="51"/>
+    </row>
+    <row r="143" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G143" s="4" t="s">
         <v>888</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K143" s="51"/>
+    </row>
+    <row r="144" spans="1:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G144" s="4" t="s">
         <v>889</v>
       </c>
-    </row>
-    <row r="145" spans="7:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="K144" s="51"/>
+    </row>
+    <row r="145" spans="7:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G145" s="4" t="s">
         <v>890</v>
       </c>
-    </row>
-    <row r="146" spans="7:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="147" spans="7:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="148" spans="7:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="149" spans="7:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="150" spans="7:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="151" spans="7:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="152" spans="7:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="153" spans="7:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="154" spans="7:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="155" spans="7:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="156" spans="7:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="157" spans="7:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="158" spans="7:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="159" spans="7:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
-    <row r="160" spans="7:7" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+      <c r="K145" s="51"/>
+    </row>
+    <row r="146" spans="7:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="147" spans="7:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="148" spans="7:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="149" spans="7:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="150" spans="7:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="151" spans="7:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="152" spans="7:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="153" spans="7:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="154" spans="7:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="155" spans="7:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="156" spans="7:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="157" spans="7:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="158" spans="7:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="159" spans="7:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="160" spans="7:11" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
     <row r="161" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
     <row r="162" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
     <row r="163" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -13932,7 +14188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>

</xml_diff>

<commit_message>
PS Excel and Rules 06/06/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Vowel Elongation" sheetId="1" r:id="rId1"/>
@@ -10846,7 +10846,7 @@
   <dimension ref="A2:N45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="M12" sqref="M12"/>
@@ -11603,11 +11603,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D102" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="D99" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="K106" sqref="K106"/>
+      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13455,11 +13455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:V294"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="E110" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="K145" sqref="K145"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15911,7 +15908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>

</xml_diff>

<commit_message>
Jatai Working files 20/06/2020 Raja
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="1"/>
   </bookViews>
   <sheets>
     <sheet name="Vowel Elongation" sheetId="1" r:id="rId1"/>
@@ -5328,9 +5328,6 @@
     <t>4.2.8.1</t>
   </si>
   <si>
-    <t xml:space="preserve"> tat | uq | soma#H |</t>
-  </si>
-  <si>
     <t>4.3.3.1</t>
   </si>
   <si>
@@ -5349,9 +5346,6 @@
     <t>4.6.2.5</t>
   </si>
   <si>
-    <t xml:space="preserve"> kaH | uq | saH |</t>
-  </si>
-  <si>
     <t>it | uq | tat | yat |</t>
   </si>
   <si>
@@ -5367,18 +5361,12 @@
     <t>5.2.12.1</t>
   </si>
   <si>
-    <t xml:space="preserve"> kaH | uq | teq | </t>
-  </si>
-  <si>
     <t>6.1.11.6</t>
   </si>
   <si>
     <t xml:space="preserve">saH | tasmA$t | uq | AqSya$m | </t>
   </si>
   <si>
-    <t xml:space="preserve"> tAsA$m | uq | tu | vai | </t>
-  </si>
-  <si>
     <t>7.5.7.1</t>
   </si>
   <si>
@@ -5425,6 +5413,18 @@
   </si>
   <si>
     <t xml:space="preserve">varca udU balam </t>
+  </si>
+  <si>
+    <t>kaH | uq | saH |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kaH | uq | teq | </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tAsA$m | uq | tu | vai | </t>
+  </si>
+  <si>
+    <t>tat | uq | soma#H |</t>
   </si>
 </sst>
 </file>
@@ -6030,8 +6030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L192"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C177" sqref="C177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11558,7 +11558,7 @@
   <dimension ref="A2:Q46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="F33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="K20" sqref="K20"/>
@@ -12378,7 +12378,7 @@
   <dimension ref="A2:Q114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="I6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
@@ -20764,8 +20764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21286,7 +21286,7 @@
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="28" t="s">
-        <v>1736</v>
+        <v>1732</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -21349,7 +21349,7 @@
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4" t="s">
-        <v>1704</v>
+        <v>1736</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -21363,14 +21363,14 @@
     </row>
     <row r="30" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>583</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -21384,14 +21384,14 @@
     </row>
     <row r="31" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>583</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -21412,7 +21412,7 @@
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -21433,7 +21433,7 @@
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -21447,14 +21447,14 @@
     </row>
     <row r="34" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>583</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4" t="s">
-        <v>1711</v>
+        <v>1733</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -21468,14 +21468,14 @@
     </row>
     <row r="35" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>583</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4" t="s">
-        <v>1712</v>
+        <v>1710</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -21489,14 +21489,14 @@
     </row>
     <row r="36" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>1713</v>
+        <v>1711</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>583</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4" t="s">
-        <v>1714</v>
+        <v>1712</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -21517,7 +21517,7 @@
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="62" t="s">
-        <v>1715</v>
+        <v>1713</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -21531,14 +21531,14 @@
     </row>
     <row r="38" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>1716</v>
+        <v>1714</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>583</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4" t="s">
-        <v>1717</v>
+        <v>1734</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
@@ -21552,14 +21552,14 @@
     </row>
     <row r="39" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>1718</v>
+        <v>1715</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>583</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4" t="s">
-        <v>1719</v>
+        <v>1716</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
@@ -21580,7 +21580,7 @@
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
-        <v>1720</v>
+        <v>1735</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
@@ -21594,14 +21594,14 @@
     </row>
     <row r="41" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>1721</v>
+        <v>1717</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>583</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4" t="s">
-        <v>1722</v>
+        <v>1718</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
@@ -21645,14 +21645,14 @@
     </row>
     <row r="44" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>1723</v>
+        <v>1719</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>304</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4" t="s">
-        <v>1724</v>
+        <v>1720</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>1695</v>
@@ -21668,12 +21668,12 @@
     </row>
     <row r="45" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>1725</v>
+        <v>1721</v>
       </c>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4" t="s">
-        <v>1726</v>
+        <v>1722</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
@@ -21687,12 +21687,12 @@
     </row>
     <row r="46" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>1727</v>
+        <v>1723</v>
       </c>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4" t="s">
-        <v>1728</v>
+        <v>1724</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
@@ -21706,12 +21706,12 @@
     </row>
     <row r="47" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>1729</v>
+        <v>1725</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4" t="s">
-        <v>1730</v>
+        <v>1726</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
@@ -21725,12 +21725,12 @@
     </row>
     <row r="48" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>1731</v>
+        <v>1727</v>
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4" t="s">
-        <v>1732</v>
+        <v>1728</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
@@ -21744,12 +21744,12 @@
     </row>
     <row r="49" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>1721</v>
+        <v>1717</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4" t="s">
-        <v>1733</v>
+        <v>1729</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
@@ -21778,12 +21778,12 @@
     </row>
     <row r="51" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>1734</v>
+        <v>1730</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4" t="s">
-        <v>1735</v>
+        <v>1731</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>

</xml_diff>

<commit_message>
Jatai Working files 24/04/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Vowel Elongation" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2916" uniqueCount="1737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2926" uniqueCount="1747">
   <si>
     <t xml:space="preserve">PrAtiSakyam Rules </t>
   </si>
@@ -5425,6 +5425,36 @@
   </si>
   <si>
     <t>tat | uq | soma#H |</t>
+  </si>
+  <si>
+    <t>Padam</t>
+  </si>
+  <si>
+    <t>SamhitA text</t>
+  </si>
+  <si>
+    <t>idamunaH</t>
+  </si>
+  <si>
+    <t>vayamutvA</t>
+  </si>
+  <si>
+    <t>sedu hotA</t>
+  </si>
+  <si>
+    <t>udutyam</t>
+  </si>
+  <si>
+    <t>asmABirU nu</t>
+  </si>
+  <si>
+    <t>idamu naH</t>
+  </si>
+  <si>
+    <t>mahimU shu mAtaram</t>
+  </si>
+  <si>
+    <t>Rutena vyu tritaH</t>
   </si>
 </sst>
 </file>
@@ -6030,7 +6060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L192"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C177" sqref="C177"/>
     </sheetView>
   </sheetViews>
@@ -11558,7 +11588,7 @@
   <dimension ref="A2:Q46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="F33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="K20" sqref="K20"/>
@@ -12378,7 +12408,7 @@
   <dimension ref="A2:Q114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D111" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
@@ -14382,7 +14412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:U294"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" workbookViewId="0">
+    <sheetView topLeftCell="A136" workbookViewId="0">
       <selection activeCell="J112" sqref="J112"/>
     </sheetView>
   </sheetViews>
@@ -17028,10 +17058,10 @@
   <dimension ref="A2:R109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C99" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C97" sqref="C97"/>
+      <selection pane="bottomRight" activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20764,8 +20794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M60"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20779,9 +20809,13 @@
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>1737</v>
+      </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>1738</v>
+      </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -20817,7 +20851,9 @@
         <v>1664</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>1739</v>
+      </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -20838,7 +20874,9 @@
         <v>1666</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>1740</v>
+      </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -20859,7 +20897,9 @@
         <v>1667</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>1741</v>
+      </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -20882,7 +20922,9 @@
       <c r="E7" s="4" t="s">
         <v>1695</v>
       </c>
-      <c r="F7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>1742</v>
+      </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -20903,7 +20945,9 @@
         <v>1669</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>1743</v>
+      </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -20924,7 +20968,9 @@
         <v>1664</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>1744</v>
+      </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -20945,7 +20991,9 @@
         <v>1670</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="F10" s="4" t="s">
+        <v>1745</v>
+      </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -20966,7 +21014,9 @@
         <v>1673</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>1746</v>
+      </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>

</xml_diff>

<commit_message>
TS Jatai Working files 25/06/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2926" uniqueCount="1747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3009" uniqueCount="1825">
   <si>
     <t xml:space="preserve">PrAtiSakyam Rules </t>
   </si>
@@ -5217,27 +5217,15 @@
     <t>vaqyam | uq | tvAq |</t>
   </si>
   <si>
-    <t>saH | it | uq | hotA$ |</t>
-  </si>
-  <si>
-    <t>ut | uq | tyam | jAqtave#dasam</t>
-  </si>
-  <si>
     <t>aqsmABi#H | uq | nu | praqtiqcakShyA$ |</t>
   </si>
   <si>
-    <t>maqhIm | uq | su | mAqtara$m |</t>
-  </si>
-  <si>
     <t>1.5.11.5</t>
   </si>
   <si>
     <t>1.8.10.2</t>
   </si>
   <si>
-    <t>Rutena | vi | u | tritaH |</t>
-  </si>
-  <si>
     <t>vAqmam | uq | SvaH |</t>
   </si>
   <si>
@@ -5247,9 +5235,6 @@
     <t>2.2.12.8</t>
   </si>
   <si>
-    <t xml:space="preserve"> pra | it | uq | haqriqvaH | </t>
-  </si>
-  <si>
     <t>aqdanti# | uq | eqva | aqsyaq |</t>
   </si>
   <si>
@@ -5259,15 +5244,9 @@
     <t xml:space="preserve">tam | uq | Suci$m | </t>
   </si>
   <si>
-    <t xml:space="preserve">kam | uq | sviqtq | aqsyaq | </t>
-  </si>
-  <si>
     <t>3.1.4.4</t>
   </si>
   <si>
-    <t xml:space="preserve">tvAm | uq | te | daqdhiqreq | </t>
-  </si>
-  <si>
     <t>saH | uq | pAqtuq |</t>
   </si>
   <si>
@@ -5280,9 +5259,6 @@
     <t>3.5.5.1</t>
   </si>
   <si>
-    <t>aqntari#kSham | tat | uq | meq |</t>
-  </si>
-  <si>
     <t>sam | ata#H | uq | su | madhu# |</t>
   </si>
   <si>
@@ -5322,9 +5298,6 @@
     <t>4.2.7.4</t>
   </si>
   <si>
-    <t>sam | uq | yaqntuq | vAjA$H |</t>
-  </si>
-  <si>
     <t>4.2.8.1</t>
   </si>
   <si>
@@ -5364,9 +5337,6 @@
     <t>6.1.11.6</t>
   </si>
   <si>
-    <t xml:space="preserve">saH | tasmA$t | uq | AqSya$m | </t>
-  </si>
-  <si>
     <t>7.5.7.1</t>
   </si>
   <si>
@@ -5448,13 +5418,277 @@
     <t>asmABirU nu</t>
   </si>
   <si>
-    <t>idamu naH</t>
-  </si>
-  <si>
-    <t>mahimU shu mAtaram</t>
-  </si>
-  <si>
     <t>Rutena vyu tritaH</t>
+  </si>
+  <si>
+    <t>Ref</t>
+  </si>
+  <si>
+    <t>pretu</t>
+  </si>
+  <si>
+    <t>adantyu veva</t>
+  </si>
+  <si>
+    <t>tamU Sucim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kam u Shvit </t>
+  </si>
+  <si>
+    <t>tvamu te</t>
+  </si>
+  <si>
+    <t>sa u pAtu</t>
+  </si>
+  <si>
+    <t>veru tat</t>
+  </si>
+  <si>
+    <t>tadu me</t>
+  </si>
+  <si>
+    <t>samata U Shu</t>
+  </si>
+  <si>
+    <t>ayamu Sya pra</t>
+  </si>
+  <si>
+    <t>sva u loke</t>
+  </si>
+  <si>
+    <t>udu tiShTha</t>
+  </si>
+  <si>
+    <t>udu tvA</t>
+  </si>
+  <si>
+    <t>samu yantu</t>
+  </si>
+  <si>
+    <t>tadu soma</t>
+  </si>
+  <si>
+    <t>u vekavi(gm)Savartanih</t>
+  </si>
+  <si>
+    <t>u pa~jcadaSavartaniH</t>
+  </si>
+  <si>
+    <t>u saptadaSavartaniH</t>
+  </si>
+  <si>
+    <t>tasAmu yanti</t>
+  </si>
+  <si>
+    <t>ka u sa</t>
+  </si>
+  <si>
+    <t>idu tat</t>
+  </si>
+  <si>
+    <t>na vA u vetat</t>
+  </si>
+  <si>
+    <t>etA u va</t>
+  </si>
+  <si>
+    <t>ka u te</t>
+  </si>
+  <si>
+    <t>tasmAdu-vAsyam</t>
+  </si>
+  <si>
+    <t>tasAmu tvA</t>
+  </si>
+  <si>
+    <t>taduvAhuH</t>
+  </si>
+  <si>
+    <t>EL</t>
+  </si>
+  <si>
+    <t>vasatu nu na idam</t>
+  </si>
+  <si>
+    <t>Jatai</t>
+  </si>
+  <si>
+    <t>Ghanam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asmABiruvuvasmABirasmABiru </t>
+  </si>
+  <si>
+    <t>asmABiruvuvasmABirasmABirUnunvasmABirasmABirUnu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adantyuvuvadantya dantyuvevaivodantyadantyuveva </t>
+  </si>
+  <si>
+    <t>adantyuvuvadantyadantyu</t>
+  </si>
+  <si>
+    <t>UtutUtu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UtutUtvaivai tUtvai </t>
+  </si>
+  <si>
+    <t>u+tu ,EL applies so becomes U; Noted merger of tu+u+u into long anyhow it will be due to elongation rule. No v added between u+u as it is followed by Consonant</t>
+  </si>
+  <si>
+    <t>mahimU Shu mAtaram</t>
+  </si>
+  <si>
+    <t>samato &amp;taH sa(gm) samata u</t>
+  </si>
+  <si>
+    <t>4.1.14.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saH | it | uq | </t>
+  </si>
+  <si>
+    <t>seditsaseduvuvitsasedu</t>
+  </si>
+  <si>
+    <t>seditsaset</t>
+  </si>
+  <si>
+    <t>iduvuvididuta ttadvidutat</t>
+  </si>
+  <si>
+    <t>iduvuvididu</t>
+  </si>
+  <si>
+    <t>iduvuvididuhotA hota vididuhotA</t>
+  </si>
+  <si>
+    <t>uq | eqva | aqsyaq |</t>
+  </si>
+  <si>
+    <t>uvevAsya</t>
+  </si>
+  <si>
+    <t>uvevaivavuvevAsyAsyaivavuvevAsya</t>
+  </si>
+  <si>
+    <t>uvevaivavuveva</t>
+  </si>
+  <si>
+    <t>sa^^uvusasa^^u pAtupAtuvsa sa upAtu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sa^^uvusasa^^u </t>
+  </si>
+  <si>
+    <t>5.3.4.7</t>
+  </si>
+  <si>
+    <t>uq | caq | eqnAqM |</t>
+  </si>
+  <si>
+    <t>ucainAm</t>
+  </si>
+  <si>
+    <t>ucacavuvucainamenaMcavucainam</t>
+  </si>
+  <si>
+    <t>ucacauvuvuca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tasmA$t | uq | AqSya$m | </t>
+  </si>
+  <si>
+    <t>tasmAdUtasmAttasmAdu</t>
+  </si>
+  <si>
+    <t>tasmAdUtasmAttasmAduvAsyamAsyamutasmattasmAtuvAsyam</t>
+  </si>
+  <si>
+    <t>tat | uq | meq |</t>
+  </si>
+  <si>
+    <t>tadUtattadu</t>
+  </si>
+  <si>
+    <t>tadUtattadu me ma u tatadu me</t>
+  </si>
+  <si>
+    <t>vayamUvayamvayamu</t>
+  </si>
+  <si>
+    <t>vayamUvayamvayamutvAtvauvayamutvA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sam | uq | yaqntuq | </t>
+  </si>
+  <si>
+    <t>samuvusamuyantuyantUsa(gm)samutvA</t>
+  </si>
+  <si>
+    <t>samato &amp;taH sa(gm) samata u vuvataH sa(gm) samata u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ut | uq | tyam | </t>
+  </si>
+  <si>
+    <t xml:space="preserve">uduvuvududutyantyamuvududutyam </t>
+  </si>
+  <si>
+    <t>uduvuvududu</t>
+  </si>
+  <si>
+    <t>idamuvuvidamidamu</t>
+  </si>
+  <si>
+    <t>uq | su | mAqtara$m |</t>
+  </si>
+  <si>
+    <t>UShusUShu</t>
+  </si>
+  <si>
+    <t>UShusUShu mAtaram mAtara(gm) sU Shu mAtaram</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vi | u | tritaH |</t>
+  </si>
+  <si>
+    <t>vyuvuvivyu</t>
+  </si>
+  <si>
+    <t>vAmamu SvaH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vAmamu vu vAmam vAmamu </t>
+  </si>
+  <si>
+    <t>vAmamu vu vAmam vAmamu ShvaH  Shva u vAmam vAmamu ShvaH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pra | it | uq |</t>
+  </si>
+  <si>
+    <t>predit prapret</t>
+  </si>
+  <si>
+    <t>predit prapretuvuvitprapretu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kam | uq | sviqtq </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tvAm | uq | te | </t>
+  </si>
+  <si>
+    <t>tamu tvA</t>
+  </si>
+  <si>
+    <t>tamUtamtamutvAtvavtamtamutvA</t>
+  </si>
+  <si>
+    <t>it | uq | hotA$ |</t>
   </si>
 </sst>
 </file>
@@ -5657,7 +5891,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -5680,11 +5914,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5777,6 +6024,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -20792,39 +21048,49 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M60"/>
+  <dimension ref="A2:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.21875" customWidth="1"/>
+    <col min="3" max="3" width="64.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" customWidth="1"/>
+    <col min="6" max="6" width="44.6640625" customWidth="1"/>
+    <col min="7" max="7" width="63.33203125" customWidth="1"/>
+    <col min="8" max="8" width="43.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
-        <v>1737</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
-        <v>1738</v>
-      </c>
-      <c r="G2" s="4"/>
+    <row r="2" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A2" s="63" t="s">
+        <v>1735</v>
+      </c>
+      <c r="B2" s="63" t="s">
+        <v>818</v>
+      </c>
+      <c r="C2" s="63" t="s">
+        <v>1727</v>
+      </c>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
+        <v>1728</v>
+      </c>
+      <c r="F2" s="64" t="s">
+        <v>1765</v>
+      </c>
+      <c r="G2" s="64" t="s">
+        <v>1766</v>
+      </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-    </row>
-    <row r="3" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -20837,22 +21103,23 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>1663</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>1664</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>1729</v>
+      </c>
       <c r="F4" s="4" t="s">
-        <v>1739</v>
+        <v>1808</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -20860,139 +21127,157 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-    </row>
-    <row r="5" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>1665</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>1666</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>1730</v>
+      </c>
       <c r="F5" s="4" t="s">
-        <v>1740</v>
-      </c>
-      <c r="G5" s="4"/>
+        <v>1800</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>1801</v>
+      </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-    </row>
-    <row r="6" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>904</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4" t="s">
-        <v>1667</v>
-      </c>
-      <c r="E6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>1824</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>1731</v>
+      </c>
       <c r="F6" s="4" t="s">
-        <v>1741</v>
-      </c>
-      <c r="G6" s="4"/>
+        <v>1781</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>1782</v>
+      </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-    </row>
-    <row r="7" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>1178</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>1805</v>
+      </c>
       <c r="D7" s="4" t="s">
-        <v>1668</v>
+        <v>1687</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>1695</v>
+        <v>1732</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>1742</v>
-      </c>
-      <c r="G7" s="4"/>
+        <v>1807</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>1806</v>
+      </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-    </row>
-    <row r="8" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>1266</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>1667</v>
+      </c>
       <c r="D8" s="4" t="s">
-        <v>1669</v>
-      </c>
-      <c r="E8" s="4"/>
+        <v>1763</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>1733</v>
+      </c>
       <c r="F8" s="4" t="s">
-        <v>1743</v>
-      </c>
-      <c r="G8" s="4"/>
+        <v>1767</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>1768</v>
+      </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-    </row>
-    <row r="9" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>981</v>
+        <v>1668</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4" t="s">
-        <v>1664</v>
-      </c>
-      <c r="E9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>1809</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>1774</v>
+      </c>
       <c r="F9" s="4" t="s">
-        <v>1744</v>
-      </c>
-      <c r="G9" s="4"/>
+        <v>1810</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>1811</v>
+      </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-    </row>
-    <row r="10" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>1671</v>
+        <v>1669</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4" t="s">
-        <v>1670</v>
-      </c>
-      <c r="E10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>1812</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>1734</v>
+      </c>
       <c r="F10" s="4" t="s">
-        <v>1745</v>
+        <v>1813</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -21000,106 +21285,127 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-    </row>
-    <row r="11" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4" t="s">
-        <v>1673</v>
-      </c>
-      <c r="E11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>1670</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>1814</v>
+      </c>
       <c r="F11" s="4" t="s">
-        <v>1746</v>
-      </c>
-      <c r="G11" s="4"/>
+        <v>1815</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>1816</v>
+      </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-    </row>
-    <row r="12" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>1675</v>
+        <v>1672</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4" t="s">
-        <v>1674</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>1817</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>1736</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>1818</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>1819</v>
+      </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-    </row>
-    <row r="13" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>1676</v>
+        <v>1585</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4" t="s">
-        <v>1677</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>1673</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>1737</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>1770</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>1769</v>
+      </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-    </row>
-    <row r="14" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>1585</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4" t="s">
-        <v>1678</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>1783</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>1784</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>1786</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>1785</v>
+      </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-    </row>
-    <row r="15" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>1679</v>
+        <v>1674</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>1675</v>
+      </c>
       <c r="D15" s="4" t="s">
-        <v>1680</v>
-      </c>
-      <c r="E15" s="4"/>
+        <v>1763</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>1738</v>
+      </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -21107,20 +21413,21 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-    </row>
-    <row r="16" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>992</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4" t="s">
-        <v>1681</v>
-      </c>
-      <c r="E16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>1820</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>1739</v>
+      </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -21128,20 +21435,21 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-    </row>
-    <row r="17" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>1682</v>
+        <v>1676</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4" t="s">
-        <v>1683</v>
-      </c>
-      <c r="E17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>1821</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>1740</v>
+      </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
@@ -21149,41 +21457,47 @@
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-    </row>
-    <row r="18" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>994</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4" t="s">
-        <v>1684</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>1741</v>
+      </c>
+      <c r="F18" s="65" t="s">
+        <v>1788</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>1787</v>
+      </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-    </row>
-    <row r="19" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>1685</v>
+        <v>1678</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4" t="s">
-        <v>1686</v>
-      </c>
-      <c r="E19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>1679</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>1742</v>
+      </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
@@ -21191,62 +21505,73 @@
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-    </row>
-    <row r="20" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>1687</v>
+        <v>1680</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4" t="s">
-        <v>1688</v>
-      </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="C20" s="4" t="s">
+        <v>1797</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4" t="s">
+        <v>1743</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>1798</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>1799</v>
+      </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-    </row>
-    <row r="21" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>1658</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="62" t="s">
-        <v>1689</v>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+      <c r="C21" s="62" t="s">
+        <v>1681</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>1744</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>1775</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>1804</v>
+      </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-    </row>
-    <row r="22" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>987</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4" t="s">
-        <v>1690</v>
-      </c>
-      <c r="E22" s="4"/>
+      <c r="C22" s="4" t="s">
+        <v>1682</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>1745</v>
+      </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -21254,21 +21579,22 @@
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-    </row>
-    <row r="23" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>1691</v>
+        <v>1683</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>1684</v>
+      </c>
       <c r="D23" s="4" t="s">
-        <v>1692</v>
+        <v>1687</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>1695</v>
+        <v>1746</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -21277,43 +21603,47 @@
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-    </row>
-    <row r="24" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>1693</v>
+        <v>1685</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C24" s="4"/>
+      <c r="C24" s="4" t="s">
+        <v>1686</v>
+      </c>
       <c r="D24" s="4" t="s">
-        <v>1694</v>
+        <v>1687</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>1695</v>
-      </c>
-      <c r="F24" s="4"/>
+        <v>1822</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>1823</v>
+      </c>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-    </row>
-    <row r="25" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>1696</v>
+        <v>1688</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4" t="s">
-        <v>1697</v>
-      </c>
-      <c r="E25" s="4"/>
+      <c r="C25" s="4" t="s">
+        <v>1689</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4" t="s">
+        <v>1747</v>
+      </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -21321,66 +21651,71 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-    </row>
-    <row r="26" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>932</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C26" s="4"/>
+      <c r="C26" s="4" t="s">
+        <v>1690</v>
+      </c>
       <c r="D26" s="4" t="s">
-        <v>1698</v>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="28" t="s">
-        <v>1732</v>
-      </c>
+        <v>1763</v>
+      </c>
+      <c r="E26" s="38" t="s">
+        <v>1722</v>
+      </c>
+      <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-    </row>
-    <row r="27" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>1699</v>
+        <v>1776</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4" t="s">
-        <v>1700</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>1695</v>
-      </c>
-      <c r="F27" s="4"/>
+      <c r="C27" s="4" t="s">
+        <v>1777</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="53" t="s">
+        <v>1779</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>1778</v>
+      </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-    </row>
-    <row r="28" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>1701</v>
+        <v>1691</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C28" s="4"/>
+      <c r="C28" s="4" t="s">
+        <v>1692</v>
+      </c>
       <c r="D28" s="4" t="s">
-        <v>1702</v>
-      </c>
-      <c r="E28" s="4"/>
+        <v>1687</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>1748</v>
+      </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -21388,41 +21723,45 @@
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-    </row>
-    <row r="29" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>1703</v>
+        <v>1693</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4" t="s">
-        <v>1736</v>
-      </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
+      <c r="C29" s="4" t="s">
+        <v>1802</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4" t="s">
+        <v>1749</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>1803</v>
+      </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-    </row>
-    <row r="30" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>1704</v>
+        <v>1694</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4" t="s">
-        <v>1705</v>
-      </c>
-      <c r="E30" s="4"/>
+      <c r="C30" s="4" t="s">
+        <v>1726</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4" t="s">
+        <v>1750</v>
+      </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
@@ -21430,20 +21769,21 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-    </row>
-    <row r="31" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>1704</v>
+        <v>1695</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4" t="s">
-        <v>1706</v>
-      </c>
-      <c r="E31" s="4"/>
+      <c r="C31" s="4" t="s">
+        <v>1696</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4" t="s">
+        <v>1752</v>
+      </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
@@ -21451,20 +21791,21 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-    </row>
-    <row r="32" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>1359</v>
+        <v>1695</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4" t="s">
-        <v>1707</v>
-      </c>
-      <c r="E32" s="4"/>
+      <c r="C32" s="4" t="s">
+        <v>1697</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4" t="s">
+        <v>1753</v>
+      </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
@@ -21472,20 +21813,21 @@
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-    </row>
-    <row r="33" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>1233</v>
+        <v>1359</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4" t="s">
-        <v>1708</v>
-      </c>
-      <c r="E33" s="4"/>
+      <c r="C33" s="4" t="s">
+        <v>1698</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4" t="s">
+        <v>1751</v>
+      </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
@@ -21493,20 +21835,21 @@
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-    </row>
-    <row r="34" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>1709</v>
+        <v>1233</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4" t="s">
-        <v>1733</v>
-      </c>
-      <c r="E34" s="4"/>
+      <c r="C34" s="4" t="s">
+        <v>1699</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4" t="s">
+        <v>1754</v>
+      </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
@@ -21514,20 +21857,21 @@
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-    </row>
-    <row r="35" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>1709</v>
+        <v>1700</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4" t="s">
-        <v>1710</v>
-      </c>
-      <c r="E35" s="4"/>
+      <c r="C35" s="4" t="s">
+        <v>1723</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4" t="s">
+        <v>1755</v>
+      </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
@@ -21535,41 +21879,47 @@
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-    </row>
-    <row r="36" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>1711</v>
+        <v>1700</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4" t="s">
-        <v>1712</v>
-      </c>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
+      <c r="C36" s="4" t="s">
+        <v>1701</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4" t="s">
+        <v>1756</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>1781</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>1780</v>
+      </c>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-    </row>
-    <row r="37" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>1197</v>
+        <v>1702</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="62" t="s">
-        <v>1713</v>
-      </c>
-      <c r="E37" s="4"/>
+      <c r="C37" s="4" t="s">
+        <v>1703</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4" t="s">
+        <v>1757</v>
+      </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
@@ -21577,20 +21927,21 @@
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-    </row>
-    <row r="38" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>1714</v>
+        <v>1197</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4" t="s">
-        <v>1734</v>
-      </c>
-      <c r="E38" s="4"/>
+      <c r="C38" s="62" t="s">
+        <v>1704</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4" t="s">
+        <v>1758</v>
+      </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
@@ -21598,20 +21949,21 @@
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-    </row>
-    <row r="39" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>1715</v>
+        <v>1705</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4" t="s">
-        <v>1716</v>
-      </c>
-      <c r="E39" s="4"/>
+      <c r="C39" s="4" t="s">
+        <v>1724</v>
+      </c>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4" t="s">
+        <v>1759</v>
+      </c>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
@@ -21619,71 +21971,101 @@
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-    </row>
-    <row r="40" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>996</v>
+        <v>1789</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4" t="s">
-        <v>1735</v>
-      </c>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
+      <c r="C40" s="15" t="s">
+        <v>1790</v>
+      </c>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4" t="s">
+        <v>1791</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>1793</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>1792</v>
+      </c>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-    </row>
-    <row r="41" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>1717</v>
+        <v>1706</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4" t="s">
-        <v>1718</v>
-      </c>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
+      <c r="C41" s="4" t="s">
+        <v>1794</v>
+      </c>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4" t="s">
+        <v>1760</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>1795</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>1796</v>
+      </c>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-    </row>
-    <row r="42" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
+    </row>
+    <row r="42" spans="1:12" ht="87" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>1725</v>
+      </c>
       <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
+      <c r="E42" s="4" t="s">
+        <v>1761</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>1771</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>1772</v>
+      </c>
+      <c r="H42" s="61" t="s">
+        <v>1773</v>
+      </c>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
-    </row>
-    <row r="43" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
+    </row>
+    <row r="43" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>1707</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>1708</v>
+      </c>
       <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
+      <c r="E43" s="4" t="s">
+        <v>1762</v>
+      </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
@@ -21691,22 +22073,13 @@
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
-      <c r="M43" s="4"/>
-    </row>
-    <row r="44" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>304</v>
-      </c>
+    </row>
+    <row r="44" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
       <c r="C44" s="4"/>
-      <c r="D44" s="4" t="s">
-        <v>1720</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>1695</v>
-      </c>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
@@ -21714,17 +22087,12 @@
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
-    </row>
-    <row r="45" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
-        <v>1721</v>
-      </c>
+    </row>
+    <row r="45" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
-      <c r="D45" s="4" t="s">
-        <v>1722</v>
-      </c>
+      <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
@@ -21733,16 +22101,19 @@
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
       <c r="L45" s="4"/>
-      <c r="M45" s="4"/>
-    </row>
-    <row r="46" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>1723</v>
-      </c>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
+        <v>1709</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>1710</v>
+      </c>
       <c r="D46" s="4" t="s">
-        <v>1724</v>
+        <v>1687</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
@@ -21752,17 +22123,16 @@
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
-    </row>
-    <row r="47" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>1725</v>
+        <v>1711</v>
       </c>
       <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4" t="s">
-        <v>1726</v>
-      </c>
+      <c r="C47" s="4" t="s">
+        <v>1712</v>
+      </c>
+      <c r="D47" s="4"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
@@ -21771,17 +22141,16 @@
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-    </row>
-    <row r="48" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>1727</v>
+        <v>1713</v>
       </c>
       <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4" t="s">
-        <v>1728</v>
-      </c>
+      <c r="C48" s="4" t="s">
+        <v>1714</v>
+      </c>
+      <c r="D48" s="4"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
@@ -21790,17 +22159,16 @@
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-    </row>
-    <row r="49" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>1717</v>
+        <v>1715</v>
       </c>
       <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4" t="s">
-        <v>1729</v>
-      </c>
+      <c r="C49" s="4" t="s">
+        <v>1716</v>
+      </c>
+      <c r="D49" s="4"/>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
@@ -21809,12 +22177,15 @@
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-    </row>
-    <row r="50" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A50" s="4"/>
+    </row>
+    <row r="50" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>1717</v>
+      </c>
       <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
+      <c r="C50" s="4" t="s">
+        <v>1718</v>
+      </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
@@ -21824,17 +22195,16 @@
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
-    </row>
-    <row r="51" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>1730</v>
+        <v>1707</v>
       </c>
       <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4" t="s">
-        <v>1731</v>
-      </c>
+      <c r="C51" s="4" t="s">
+        <v>1719</v>
+      </c>
+      <c r="D51" s="4"/>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
@@ -21843,9 +22213,8 @@
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
-      <c r="M51" s="4"/>
-    </row>
-    <row r="52" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -21858,14 +22227,19 @@
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
-      <c r="M52" s="4"/>
-    </row>
-    <row r="53" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A53" s="4"/>
+    </row>
+    <row r="53" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>1720</v>
+      </c>
       <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
+      <c r="C53" s="4" t="s">
+        <v>1721</v>
+      </c>
       <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
+      <c r="E53" s="4" t="s">
+        <v>1764</v>
+      </c>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
@@ -21873,9 +22247,8 @@
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
-    </row>
-    <row r="54" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -21888,9 +22261,8 @@
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
-    </row>
-    <row r="55" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -21903,9 +22275,8 @@
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
-    </row>
-    <row r="56" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -21918,9 +22289,8 @@
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
-      <c r="M56" s="4"/>
-    </row>
-    <row r="57" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -21933,9 +22303,8 @@
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
-      <c r="M57" s="4"/>
-    </row>
-    <row r="58" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -21948,9 +22317,8 @@
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
-      <c r="M58" s="4"/>
-    </row>
-    <row r="59" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -21963,9 +22331,8 @@
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
-      <c r="M59" s="4"/>
-    </row>
-    <row r="60" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -21978,10 +22345,37 @@
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
-      <c r="M60" s="4"/>
+    </row>
+    <row r="61" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="4"/>
+      <c r="L61" s="4"/>
+    </row>
+    <row r="62" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="4"/>
+      <c r="L62" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TS working pushed 07/07/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Vowel Elongation" sheetId="1" r:id="rId1"/>
@@ -13235,8 +13235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q114"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="G61" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="I110" sqref="I110"/>
@@ -15276,7 +15276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:U294"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
@@ -18023,7 +18023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>

</xml_diff>

<commit_message>
Changes TS Jatai working
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9192" windowHeight="2688" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Vowel Elongation" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3364" uniqueCount="2015">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3375" uniqueCount="2024">
   <si>
     <t xml:space="preserve">PrAtiSakyam Rules </t>
   </si>
@@ -5496,12 +5496,6 @@
     <t xml:space="preserve">saH | it | uq | </t>
   </si>
   <si>
-    <t>seditsaseduvuvitsasedu</t>
-  </si>
-  <si>
-    <t>seditsaset</t>
-  </si>
-  <si>
     <t>iduvuvididuta ttadvidutat</t>
   </si>
   <si>
@@ -6259,6 +6253,39 @@
   </si>
   <si>
     <t>uduvuvududutvA tvav udutvA</t>
+  </si>
+  <si>
+    <t>sedithsaset</t>
+  </si>
+  <si>
+    <t>sedithsaseduvuvithsasedu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sedu </t>
+  </si>
+  <si>
+    <t>Ghana Sandhi</t>
+  </si>
+  <si>
+    <t>Matching</t>
+  </si>
+  <si>
+    <t>hotA viduduhotA Sandhi rule A+u ??</t>
+  </si>
+  <si>
+    <t>uq | hotA$ | saH</t>
+  </si>
+  <si>
+    <t>uhotAhotavuhotA</t>
+  </si>
+  <si>
+    <t>uhotAhotavuhotA sa sa hotavuhotA saH</t>
+  </si>
+  <si>
+    <t>u hotA saH</t>
+  </si>
+  <si>
+    <t>same issue</t>
   </si>
 </sst>
 </file>
@@ -13193,7 +13220,7 @@
         <v>276</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>1807</v>
+        <v>1805</v>
       </c>
       <c r="I40" s="4" t="s">
         <v>1213</v>
@@ -13235,7 +13262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -13683,13 +13710,13 @@
         <v>1636</v>
       </c>
       <c r="J30" s="4" t="s">
+        <v>1806</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>1807</v>
+      </c>
+      <c r="M30" s="4" t="s">
         <v>1808</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>1809</v>
-      </c>
-      <c r="M30" s="4" t="s">
-        <v>1810</v>
       </c>
       <c r="P30" s="32" t="s">
         <v>1147</v>
@@ -14234,7 +14261,7 @@
         <v>1222</v>
       </c>
       <c r="O58" s="4" t="s">
-        <v>1811</v>
+        <v>1809</v>
       </c>
     </row>
     <row r="59" spans="1:15" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -16774,7 +16801,7 @@
         <v>1376</v>
       </c>
       <c r="Q92" s="32" t="s">
-        <v>1812</v>
+        <v>1810</v>
       </c>
       <c r="R92" s="58" t="s">
         <v>1377</v>
@@ -16783,7 +16810,7 @@
         <v>1378</v>
       </c>
       <c r="T92" s="4" t="s">
-        <v>1813</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="93" spans="1:20" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -16805,7 +16832,7 @@
       </c>
       <c r="L94" s="39"/>
       <c r="M94" s="4" t="s">
-        <v>1814</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="95" spans="1:20" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -17302,7 +17329,7 @@
         <v>896</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>1816</v>
+        <v>1814</v>
       </c>
       <c r="D115" s="4" t="s">
         <v>276</v>
@@ -17317,7 +17344,7 @@
         <v>898</v>
       </c>
       <c r="I115" s="59" t="s">
-        <v>1815</v>
+        <v>1813</v>
       </c>
       <c r="J115" s="59" t="s">
         <v>900</v>
@@ -18096,28 +18123,28 @@
         <v>359</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>1817</v>
+        <v>1815</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>515</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>1821</v>
+        <v>1819</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>1819</v>
+        <v>1817</v>
       </c>
       <c r="L6" s="32" t="s">
         <v>1147</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>1820</v>
+        <v>1818</v>
       </c>
       <c r="O6" s="4" t="s">
         <v>515</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>1818</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="7" spans="1:22" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -18126,22 +18153,22 @@
         <v>2</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>1822</v>
+        <v>1820</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>359</v>
       </c>
       <c r="G7" s="4" t="s">
+        <v>1821</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>1820</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>1822</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>1823</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>1822</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>1824</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>1825</v>
       </c>
       <c r="L7" s="32" t="s">
         <v>1147</v>
@@ -18165,10 +18192,10 @@
         <v>472</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>1826</v>
+        <v>1824</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>1827</v>
+        <v>1825</v>
       </c>
       <c r="L8" s="32" t="s">
         <v>1147</v>
@@ -18186,34 +18213,34 @@
         <v>359</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>1828</v>
+        <v>1826</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>516</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>1829</v>
+        <v>1827</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>1830</v>
+        <v>1828</v>
       </c>
       <c r="L9" s="32" t="s">
         <v>1147</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>1831</v>
+        <v>1829</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>1832</v>
+        <v>1830</v>
       </c>
       <c r="P9" s="4" t="s">
         <v>516</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>1833</v>
+        <v>1831</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>1834</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="10" spans="1:22" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -18222,7 +18249,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>1835</v>
+        <v>1833</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>359</v>
@@ -18231,22 +18258,22 @@
         <v>85</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>1835</v>
+        <v>1833</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>1835</v>
+        <v>1833</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>1838</v>
+        <v>1836</v>
       </c>
       <c r="L10" s="32" t="s">
         <v>1147</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>1836</v>
+        <v>1834</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>1837</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="11" spans="1:22" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -18267,10 +18294,10 @@
         <v>519</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>1839</v>
+        <v>1837</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>1840</v>
+        <v>1838</v>
       </c>
       <c r="L11" s="32" t="s">
         <v>1147</v>
@@ -18294,10 +18321,10 @@
         <v>520</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>1841</v>
+        <v>1839</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>1842</v>
+        <v>1840</v>
       </c>
       <c r="L12" s="32" t="s">
         <v>1147</v>
@@ -18324,40 +18351,40 @@
         <v>749</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>1843</v>
+        <v>1841</v>
       </c>
       <c r="L13" s="32" t="s">
         <v>1147</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>1848</v>
+        <v>1846</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>517</v>
       </c>
       <c r="O13" s="4" t="s">
+        <v>1847</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>1848</v>
+      </c>
+      <c r="Q13" s="4" t="s">
         <v>1849</v>
       </c>
-      <c r="P13" s="4" t="s">
+      <c r="R13" s="4" t="s">
         <v>1850</v>
-      </c>
-      <c r="Q13" s="4" t="s">
-        <v>1851</v>
-      </c>
-      <c r="R13" s="4" t="s">
-        <v>1852</v>
       </c>
       <c r="S13" s="4" t="s">
         <v>931</v>
       </c>
       <c r="T13" s="4" t="s">
-        <v>1853</v>
+        <v>1851</v>
       </c>
       <c r="U13" s="4" t="s">
         <v>933</v>
       </c>
       <c r="V13" s="4" t="s">
-        <v>1854</v>
+        <v>1852</v>
       </c>
     </row>
     <row r="14" spans="1:22" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -18375,25 +18402,25 @@
         <v>1173</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>1846</v>
+        <v>1844</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>1844</v>
+        <v>1842</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>1855</v>
+        <v>1853</v>
       </c>
       <c r="L14" s="32" t="s">
         <v>1147</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>1845</v>
+        <v>1843</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>521</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>1847</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="15" spans="1:22" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -18426,7 +18453,7 @@
         <v>359</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="L16" s="32" t="s">
         <v>1147</v>
@@ -18453,7 +18480,7 @@
         <v>749</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>1856</v>
+        <v>1854</v>
       </c>
       <c r="L17" s="32" t="s">
         <v>1147</v>
@@ -18477,10 +18504,10 @@
         <v>522</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>1857</v>
+        <v>1855</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>1858</v>
+        <v>1856</v>
       </c>
       <c r="L18" s="32" t="s">
         <v>1147</v>
@@ -18504,10 +18531,10 @@
         <v>523</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>1859</v>
+        <v>1857</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>1860</v>
+        <v>1858</v>
       </c>
       <c r="L19" s="32" t="s">
         <v>1147</v>
@@ -18519,28 +18546,28 @@
         <v>15</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>1865</v>
+        <v>1863</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>359</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>1864</v>
+        <v>1862</v>
       </c>
       <c r="H20" s="4" t="s">
+        <v>1859</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>1860</v>
+      </c>
+      <c r="J20" s="4" t="s">
         <v>1861</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>1862</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>1863</v>
       </c>
       <c r="L20" s="32" t="s">
         <v>1147</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>1866</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="21" spans="2:16" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -18555,7 +18582,7 @@
         <v>359</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>1867</v>
+        <v>1865</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>525</v>
@@ -18564,7 +18591,7 @@
         <v>536</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>1868</v>
+        <v>1866</v>
       </c>
       <c r="L21" s="32" t="s">
         <v>1147</v>
@@ -18582,31 +18609,31 @@
         <v>359</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>1869</v>
+        <v>1867</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>526</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>1871</v>
+        <v>1869</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>1870</v>
+        <v>1868</v>
       </c>
       <c r="L22" s="32" t="s">
         <v>1147</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>1872</v>
+        <v>1870</v>
       </c>
       <c r="N22" s="4" t="s">
         <v>526</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>1873</v>
+        <v>1871</v>
       </c>
       <c r="P22" s="4" t="s">
-        <v>1874</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="23" spans="2:16" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -18627,10 +18654,10 @@
         <v>527</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>1875</v>
+        <v>1873</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>1876</v>
+        <v>1874</v>
       </c>
       <c r="L23" s="32" t="s">
         <v>1147</v>
@@ -18657,7 +18684,7 @@
         <v>20</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>359</v>
@@ -18666,13 +18693,13 @@
         <v>1018</v>
       </c>
       <c r="H25" s="4" t="s">
+        <v>1875</v>
+      </c>
+      <c r="I25" s="4" t="s">
         <v>1877</v>
       </c>
-      <c r="I25" s="4" t="s">
-        <v>1879</v>
-      </c>
       <c r="J25" s="4" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
       <c r="L25" s="32" t="s">
         <v>1147</v>
@@ -18684,7 +18711,7 @@
         <v>21</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>1878</v>
+        <v>1876</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>359</v>
@@ -18693,28 +18720,28 @@
         <v>1035</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>1878</v>
+        <v>1876</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>1881</v>
+        <v>1879</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>1882</v>
+        <v>1880</v>
       </c>
       <c r="L26" s="32" t="s">
         <v>1147</v>
       </c>
       <c r="M26" s="4" t="s">
+        <v>1881</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>1876</v>
+      </c>
+      <c r="O26" s="4" t="s">
+        <v>1882</v>
+      </c>
+      <c r="P26" s="4" t="s">
         <v>1883</v>
-      </c>
-      <c r="N26" s="4" t="s">
-        <v>1878</v>
-      </c>
-      <c r="O26" s="4" t="s">
-        <v>1884</v>
-      </c>
-      <c r="P26" s="4" t="s">
-        <v>1885</v>
       </c>
     </row>
     <row r="27" spans="2:16" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -18729,22 +18756,22 @@
         <v>359</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>1886</v>
+        <v>1884</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>530</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>1887</v>
+        <v>1885</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>1888</v>
+        <v>1886</v>
       </c>
       <c r="L27" s="32" t="s">
         <v>1147</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>1900</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="28" spans="2:16" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -18759,7 +18786,7 @@
         <v>359</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>1889</v>
+        <v>1887</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>529</v>
@@ -18768,7 +18795,7 @@
         <v>825</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>1890</v>
+        <v>1888</v>
       </c>
       <c r="L28" s="32" t="s">
         <v>1147</v>
@@ -18786,16 +18813,16 @@
         <v>359</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>1891</v>
+        <v>1889</v>
       </c>
       <c r="H29" s="4" t="s">
         <v>533</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>1892</v>
+        <v>1890</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>1893</v>
+        <v>1891</v>
       </c>
       <c r="L29" s="32" t="s">
         <v>1147</v>
@@ -18813,16 +18840,16 @@
         <v>359</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>1894</v>
+        <v>1892</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>531</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>1905</v>
+        <v>1903</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>1895</v>
+        <v>1893</v>
       </c>
       <c r="L30" s="32" t="s">
         <v>1147</v>
@@ -18834,19 +18861,19 @@
         <v>26</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>1896</v>
+        <v>1894</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>359</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>1899</v>
+        <v>1897</v>
       </c>
       <c r="L31" s="32" t="s">
         <v>1147</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>1901</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="32" spans="2:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -18861,7 +18888,7 @@
         <v>359</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>1897</v>
+        <v>1895</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>532</v>
@@ -18870,22 +18897,22 @@
         <v>1193</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>1898</v>
+        <v>1896</v>
       </c>
       <c r="L32" s="32" t="s">
         <v>1147</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>1902</v>
+        <v>1900</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>532</v>
       </c>
       <c r="O32" s="4" t="s">
-        <v>1903</v>
+        <v>1901</v>
       </c>
       <c r="P32" s="4" t="s">
-        <v>1904</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="33" spans="1:22" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -18903,16 +18930,16 @@
         <v>359</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>1906</v>
+        <v>1904</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>1529</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>1907</v>
+        <v>1905</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>1908</v>
+        <v>1906</v>
       </c>
       <c r="L34" s="32" t="s">
         <v>1147</v>
@@ -18927,7 +18954,7 @@
         <v>1530</v>
       </c>
       <c r="P34" s="4" t="s">
-        <v>1913</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="35" spans="1:22" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -18939,28 +18966,28 @@
         <v>534</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>1909</v>
+        <v>1907</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>1910</v>
+        <v>1908</v>
       </c>
       <c r="L35" s="32" t="s">
         <v>1147</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>1911</v>
+        <v>1909</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>534</v>
       </c>
       <c r="O35" s="4" t="s">
+        <v>1910</v>
+      </c>
+      <c r="P35" s="4" t="s">
+        <v>1914</v>
+      </c>
+      <c r="Q35" s="4" t="s">
         <v>1912</v>
-      </c>
-      <c r="P35" s="4" t="s">
-        <v>1916</v>
-      </c>
-      <c r="Q35" s="4" t="s">
-        <v>1914</v>
       </c>
       <c r="R35" s="4" t="s">
         <v>534</v>
@@ -18969,13 +18996,13 @@
         <v>742</v>
       </c>
       <c r="T35" s="4" t="s">
+        <v>1913</v>
+      </c>
+      <c r="U35" s="4" t="s">
         <v>1915</v>
       </c>
-      <c r="U35" s="4" t="s">
-        <v>1917</v>
-      </c>
       <c r="V35" s="4" t="s">
-        <v>1918</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="36" spans="1:22" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -19001,13 +19028,13 @@
         <v>1020</v>
       </c>
       <c r="H38" s="4" t="s">
+        <v>1917</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>1918</v>
+      </c>
+      <c r="J38" s="4" t="s">
         <v>1919</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>1920</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>1921</v>
       </c>
       <c r="L38" s="32" t="s">
         <v>1147</v>
@@ -19051,13 +19078,13 @@
         <v>1523</v>
       </c>
       <c r="H41" s="4" t="s">
+        <v>1920</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>1921</v>
+      </c>
+      <c r="J41" s="4" t="s">
         <v>1922</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>1923</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>1924</v>
       </c>
       <c r="L41" s="32" t="s">
         <v>1147</v>
@@ -19066,13 +19093,13 @@
         <v>1523</v>
       </c>
       <c r="N41" s="4" t="s">
-        <v>1922</v>
+        <v>1920</v>
       </c>
       <c r="O41" s="4" t="s">
         <v>471</v>
       </c>
       <c r="P41" s="4" t="s">
-        <v>1925</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="42" spans="1:22" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -19088,7 +19115,7 @@
         <v>1522</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>1926</v>
+        <v>1924</v>
       </c>
       <c r="L42" s="32" t="s">
         <v>1147</v>
@@ -19096,7 +19123,7 @@
     </row>
     <row r="43" spans="1:22" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C43" s="6" t="s">
-        <v>1932</v>
+        <v>1930</v>
       </c>
       <c r="M43" s="4" t="s">
         <v>1523</v>
@@ -19140,17 +19167,17 @@
         <v>1540</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
       <c r="K44" s="53"/>
       <c r="L44" s="32" t="s">
         <v>1147</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>1928</v>
+        <v>1926</v>
       </c>
       <c r="N44" s="4" t="s">
-        <v>1929</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="45" spans="1:22" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -19171,7 +19198,7 @@
         <v>359</v>
       </c>
       <c r="G46" s="39" t="s">
-        <v>1899</v>
+        <v>1897</v>
       </c>
       <c r="H46" s="4" t="s">
         <v>1542</v>
@@ -19180,7 +19207,7 @@
         <v>536</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>1930</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="47" spans="1:22" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -19439,7 +19466,7 @@
         <v>1551</v>
       </c>
       <c r="N66" s="4" t="s">
-        <v>1964</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="67" spans="1:19" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -19562,7 +19589,7 @@
         <v>422</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>1931</v>
+        <v>1929</v>
       </c>
       <c r="J74" s="32" t="s">
         <v>1147</v>
@@ -19609,10 +19636,10 @@
         <v>1597</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>1940</v>
+        <v>1938</v>
       </c>
       <c r="I76" s="4" t="s">
-        <v>1950</v>
+        <v>1948</v>
       </c>
       <c r="J76" s="32" t="s">
         <v>1147</v>
@@ -19624,7 +19651,7 @@
         <v>1599</v>
       </c>
       <c r="P76" s="4" t="s">
-        <v>1965</v>
+        <v>1963</v>
       </c>
       <c r="Q76" s="4" t="s">
         <v>1050</v>
@@ -19635,7 +19662,7 @@
         <v>8.26</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>1975</v>
+        <v>1973</v>
       </c>
       <c r="F77" s="4" t="s">
         <v>352</v>
@@ -19679,57 +19706,57 @@
         <v>352</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>1937</v>
+        <v>1935</v>
       </c>
       <c r="H79" s="4" t="s">
-        <v>1956</v>
+        <v>1954</v>
       </c>
       <c r="I79" s="4" t="s">
-        <v>1973</v>
+        <v>1971</v>
       </c>
       <c r="J79" s="32" t="s">
         <v>1147</v>
       </c>
       <c r="K79" s="4" t="s">
-        <v>1937</v>
+        <v>1935</v>
       </c>
       <c r="L79" s="4" t="s">
+        <v>1943</v>
+      </c>
+      <c r="M79" s="4" t="s">
+        <v>1936</v>
+      </c>
+      <c r="N79" s="4" t="s">
         <v>1945</v>
-      </c>
-      <c r="M79" s="4" t="s">
-        <v>1938</v>
-      </c>
-      <c r="N79" s="4" t="s">
-        <v>1947</v>
       </c>
     </row>
     <row r="80" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E80" s="6" t="s">
-        <v>1933</v>
+        <v>1931</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>1541</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>1972</v>
+        <v>1970</v>
       </c>
       <c r="H80" s="66"/>
       <c r="I80" s="66"/>
       <c r="J80" s="6"/>
       <c r="K80" s="5" t="s">
-        <v>1936</v>
+        <v>1934</v>
       </c>
       <c r="L80" s="5" t="s">
         <v>745</v>
       </c>
       <c r="M80" s="5" t="s">
-        <v>1934</v>
+        <v>1932</v>
       </c>
       <c r="N80" s="4" t="s">
-        <v>1935</v>
+        <v>1933</v>
       </c>
       <c r="O80" s="5" t="s">
-        <v>1967</v>
+        <v>1965</v>
       </c>
       <c r="P80" s="5" t="s">
         <v>1025</v>
@@ -19738,10 +19765,10 @@
         <v>362</v>
       </c>
       <c r="R80" s="5" t="s">
-        <v>1933</v>
+        <v>1931</v>
       </c>
       <c r="S80" s="5" t="s">
-        <v>1939</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="81" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -19752,22 +19779,22 @@
         <v>352</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>1960</v>
+        <v>1958</v>
       </c>
       <c r="J81" s="32" t="s">
         <v>1147</v>
       </c>
       <c r="K81" s="4" t="s">
-        <v>1960</v>
+        <v>1958</v>
       </c>
       <c r="L81" s="4" t="s">
-        <v>1961</v>
+        <v>1959</v>
       </c>
       <c r="M81" s="4" t="s">
         <v>283</v>
       </c>
       <c r="N81" s="4" t="s">
-        <v>1962</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="82" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -19781,7 +19808,7 @@
         <v>1638</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>1951</v>
+        <v>1949</v>
       </c>
       <c r="J82" s="32" t="s">
         <v>1147</v>
@@ -19790,16 +19817,16 @@
         <v>1638</v>
       </c>
       <c r="L82" s="4" t="s">
-        <v>1941</v>
+        <v>1939</v>
       </c>
       <c r="M82" s="4" t="s">
-        <v>1942</v>
+        <v>1940</v>
       </c>
       <c r="N82" s="4" t="s">
-        <v>1948</v>
+        <v>1946</v>
       </c>
       <c r="O82" s="4" t="s">
-        <v>1949</v>
+        <v>1947</v>
       </c>
       <c r="P82" s="4" t="s">
         <v>563</v>
@@ -19807,45 +19834,45 @@
     </row>
     <row r="83" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E83" s="4" t="s">
-        <v>1943</v>
+        <v>1941</v>
       </c>
       <c r="F83" s="4" t="s">
         <v>352</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>1944</v>
+        <v>1942</v>
       </c>
       <c r="H83" s="4" t="s">
-        <v>1959</v>
+        <v>1957</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>1966</v>
+        <v>1964</v>
       </c>
       <c r="J83" s="32" t="s">
         <v>1147</v>
       </c>
       <c r="K83" s="4" t="s">
+        <v>1942</v>
+      </c>
+      <c r="L83" s="4" t="s">
+        <v>1943</v>
+      </c>
+      <c r="M83" s="4" t="s">
+        <v>1941</v>
+      </c>
+      <c r="N83" s="4" t="s">
         <v>1944</v>
-      </c>
-      <c r="L83" s="4" t="s">
-        <v>1945</v>
-      </c>
-      <c r="M83" s="4" t="s">
-        <v>1943</v>
-      </c>
-      <c r="N83" s="4" t="s">
-        <v>1946</v>
       </c>
       <c r="O83" s="4" t="s">
         <v>1169</v>
       </c>
       <c r="P83" s="4" t="s">
-        <v>1971</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="84" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E84" s="6" t="s">
-        <v>1952</v>
+        <v>1950</v>
       </c>
       <c r="F84" s="6" t="s">
         <v>1541</v>
@@ -19855,28 +19882,28 @@
       <c r="I84" s="66"/>
       <c r="J84" s="4"/>
       <c r="K84" s="5" t="s">
+        <v>1951</v>
+      </c>
+      <c r="L84" s="5" t="s">
+        <v>1952</v>
+      </c>
+      <c r="M84" s="5" t="s">
         <v>1953</v>
-      </c>
-      <c r="L84" s="5" t="s">
-        <v>1954</v>
-      </c>
-      <c r="M84" s="5" t="s">
-        <v>1955</v>
       </c>
       <c r="N84" s="4"/>
     </row>
     <row r="85" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E85" s="6" t="s">
-        <v>1957</v>
+        <v>1955</v>
       </c>
       <c r="F85" s="6" t="s">
         <v>1541</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>1958</v>
+        <v>1956</v>
       </c>
       <c r="H85" s="6" t="s">
-        <v>1974</v>
+        <v>1972</v>
       </c>
       <c r="I85" s="66"/>
       <c r="J85" s="4"/>
@@ -19887,7 +19914,7 @@
     </row>
     <row r="86" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E86" s="4" t="s">
-        <v>1963</v>
+        <v>1961</v>
       </c>
       <c r="F86" s="4" t="s">
         <v>352</v>
@@ -19906,36 +19933,36 @@
         <v>551</v>
       </c>
       <c r="M86" s="4" t="s">
-        <v>1963</v>
+        <v>1961</v>
       </c>
       <c r="N86" s="4" t="s">
-        <v>1964</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="87" spans="1:16" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="E87" s="4" t="s">
-        <v>1968</v>
+        <v>1966</v>
       </c>
       <c r="F87" s="4" t="s">
         <v>352</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>1969</v>
+        <v>1967</v>
       </c>
       <c r="J87" s="32" t="s">
         <v>1147</v>
       </c>
       <c r="K87" s="4" t="s">
-        <v>1969</v>
+        <v>1967</v>
       </c>
       <c r="L87" s="4" t="s">
         <v>299</v>
       </c>
       <c r="M87" s="4" t="s">
+        <v>1966</v>
+      </c>
+      <c r="N87" s="4" t="s">
         <v>1968</v>
-      </c>
-      <c r="N87" s="4" t="s">
-        <v>1970</v>
       </c>
     </row>
     <row r="88" spans="1:16" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -19964,7 +19991,7 @@
         <v>477</v>
       </c>
       <c r="N88" s="4" t="s">
-        <v>1976</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="89" spans="1:16" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -19987,10 +20014,10 @@
         <v>565</v>
       </c>
       <c r="M89" s="4" t="s">
-        <v>1977</v>
+        <v>1975</v>
       </c>
       <c r="N89" s="4" t="s">
-        <v>1978</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="90" spans="1:16" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -20011,10 +20038,10 @@
         <v>1019</v>
       </c>
       <c r="H91" s="4" t="s">
-        <v>1982</v>
+        <v>1980</v>
       </c>
       <c r="I91" s="4" t="s">
-        <v>1981</v>
+        <v>1979</v>
       </c>
       <c r="J91" s="32" t="s">
         <v>1147</v>
@@ -20026,10 +20053,10 @@
         <v>567</v>
       </c>
       <c r="M91" s="4" t="s">
-        <v>1979</v>
+        <v>1977</v>
       </c>
       <c r="N91" s="4" t="s">
-        <v>1980</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="92" spans="1:16" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -20046,22 +20073,22 @@
         <v>352</v>
       </c>
       <c r="G92" s="4" t="s">
-        <v>1983</v>
+        <v>1981</v>
       </c>
       <c r="J92" s="32" t="s">
         <v>1147</v>
       </c>
       <c r="K92" s="4" t="s">
-        <v>1983</v>
+        <v>1981</v>
       </c>
       <c r="L92" s="4" t="s">
         <v>299</v>
       </c>
       <c r="M92" s="4" t="s">
-        <v>1984</v>
+        <v>1982</v>
       </c>
       <c r="N92" s="4" t="s">
-        <v>1985</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="93" spans="1:16" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -20078,22 +20105,22 @@
         <v>366</v>
       </c>
       <c r="G93" s="4" t="s">
-        <v>1986</v>
+        <v>1984</v>
       </c>
       <c r="J93" s="32" t="s">
         <v>1147</v>
       </c>
       <c r="K93" s="4" t="s">
-        <v>1986</v>
+        <v>1984</v>
       </c>
       <c r="L93" s="4" t="s">
         <v>570</v>
       </c>
       <c r="M93" s="4" t="s">
-        <v>1987</v>
+        <v>1985</v>
       </c>
       <c r="N93" s="4" t="s">
-        <v>1988</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="94" spans="1:16" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -20117,7 +20144,7 @@
         <v>998</v>
       </c>
       <c r="H97" s="4" t="s">
-        <v>1989</v>
+        <v>1987</v>
       </c>
       <c r="J97" s="4" t="s">
         <v>1560</v>
@@ -20131,10 +20158,10 @@
         <v>874</v>
       </c>
       <c r="G98" s="4" t="s">
-        <v>1992</v>
+        <v>1990</v>
       </c>
       <c r="K98" s="4" t="s">
-        <v>1992</v>
+        <v>1990</v>
       </c>
       <c r="L98" s="4" t="s">
         <v>535</v>
@@ -20143,7 +20170,7 @@
         <v>280</v>
       </c>
       <c r="N98" s="4" t="s">
-        <v>1993</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="99" spans="1:15" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -20154,42 +20181,42 @@
         <v>874</v>
       </c>
       <c r="G99" s="4" t="s">
-        <v>1990</v>
+        <v>1988</v>
       </c>
       <c r="K99" s="4" t="s">
-        <v>1990</v>
+        <v>1988</v>
       </c>
       <c r="L99" s="4" t="s">
         <v>572</v>
       </c>
       <c r="M99" s="4" t="s">
-        <v>1943</v>
+        <v>1941</v>
       </c>
       <c r="N99" s="4" t="s">
-        <v>1991</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="100" spans="1:15" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C100" s="4" t="s">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="F100" s="5" t="s">
         <v>874</v>
       </c>
       <c r="G100" s="4" t="s">
+        <v>1992</v>
+      </c>
+      <c r="K100" s="4" t="s">
+        <v>1992</v>
+      </c>
+      <c r="L100" s="4" t="s">
         <v>1994</v>
       </c>
-      <c r="K100" s="4" t="s">
+      <c r="M100" s="4" t="s">
         <v>1994</v>
       </c>
-      <c r="L100" s="4" t="s">
-        <v>1996</v>
-      </c>
-      <c r="M100" s="4" t="s">
-        <v>1996</v>
-      </c>
       <c r="N100" s="4" t="s">
-        <v>1997</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="101" spans="1:15" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -20200,10 +20227,10 @@
         <v>874</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="K101" s="4" t="s">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="L101" s="4" t="s">
         <v>522</v>
@@ -20212,7 +20239,7 @@
         <v>477</v>
       </c>
       <c r="N101" s="4" t="s">
-        <v>1999</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="102" spans="1:15" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -20237,13 +20264,13 @@
         <v>8.34</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>2000</v>
+        <v>1998</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="K105" s="4" t="s">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="L105" s="4" t="s">
         <v>564</v>
@@ -20252,10 +20279,10 @@
         <v>477</v>
       </c>
       <c r="N105" s="4" t="s">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="O105" s="4" t="s">
-        <v>2003</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="106" spans="1:15" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -20263,13 +20290,13 @@
         <v>280</v>
       </c>
       <c r="G106" s="4" t="s">
+        <v>2002</v>
+      </c>
+      <c r="H106" s="4" t="s">
         <v>2004</v>
       </c>
-      <c r="H106" s="4" t="s">
-        <v>2006</v>
-      </c>
       <c r="K106" s="4" t="s">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="L106" s="4" t="s">
         <v>567</v>
@@ -20278,7 +20305,7 @@
         <v>280</v>
       </c>
       <c r="O106" s="4" t="s">
-        <v>2005</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="107" spans="1:15" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -20289,19 +20316,19 @@
         <v>412</v>
       </c>
       <c r="H107" s="4" t="s">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="K107" s="4" t="s">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="L107" s="4" t="s">
         <v>412</v>
       </c>
       <c r="M107" s="4" t="s">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="O107" s="4" t="s">
-        <v>2010</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="108" spans="1:15" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -20312,10 +20339,10 @@
         <v>412</v>
       </c>
       <c r="M108" s="4" t="s">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="O108" s="4" t="s">
-        <v>2012</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="109" spans="1:15" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -22736,10 +22763,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L62"/>
+  <dimension ref="A2:L63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22748,7 +22775,7 @@
     <col min="3" max="3" width="64.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.44140625" customWidth="1"/>
     <col min="6" max="6" width="44.6640625" customWidth="1"/>
-    <col min="7" max="7" width="63.33203125" customWidth="1"/>
+    <col min="7" max="7" width="80.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="43.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -22772,7 +22799,9 @@
       <c r="G2" s="64" t="s">
         <v>1748</v>
       </c>
-      <c r="H2" s="4"/>
+      <c r="H2" s="4" t="s">
+        <v>2016</v>
+      </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -22807,7 +22836,7 @@
         <v>1711</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>1790</v>
+        <v>1788</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -22831,10 +22860,10 @@
         <v>1712</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>1782</v>
+        <v>1780</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>1783</v>
+        <v>1781</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -22850,19 +22879,21 @@
         <v>574</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>1806</v>
+        <v>1804</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
         <v>1713</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>1763</v>
+        <v>1761</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>1764</v>
-      </c>
-      <c r="H6" s="4"/>
+        <v>1762</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>2018</v>
+      </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -22870,27 +22901,27 @@
     </row>
     <row r="7" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>1168</v>
+        <v>895</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>1787</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>1669</v>
-      </c>
+        <v>2019</v>
+      </c>
+      <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>1714</v>
+        <v>2022</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>1789</v>
+        <v>2020</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>1788</v>
-      </c>
-      <c r="H7" s="4"/>
+        <v>2021</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>2023</v>
+      </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -22898,25 +22929,25 @@
     </row>
     <row r="8" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>1256</v>
+        <v>1168</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>1649</v>
+        <v>1785</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>1745</v>
+        <v>1669</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>1749</v>
+        <v>1787</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>1750</v>
+        <v>1786</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -22926,23 +22957,25 @@
     </row>
     <row r="9" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>1650</v>
+        <v>1256</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>1791</v>
-      </c>
-      <c r="D9" s="4"/>
+        <v>1649</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>1745</v>
+      </c>
       <c r="E9" s="4" t="s">
-        <v>1756</v>
+        <v>1715</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>1792</v>
+        <v>1749</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>1793</v>
+        <v>1750</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -22952,22 +22985,24 @@
     </row>
     <row r="10" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>1794</v>
+        <v>1789</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>1716</v>
+        <v>1756</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>1795</v>
-      </c>
-      <c r="G10" s="4"/>
+        <v>1790</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>1791</v>
+      </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -22976,24 +23011,22 @@
     </row>
     <row r="11" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>1653</v>
+        <v>1651</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>1652</v>
+        <v>1792</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>1796</v>
+        <v>1716</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>1797</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>1798</v>
-      </c>
+        <v>1793</v>
+      </c>
+      <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
@@ -23002,23 +23035,23 @@
     </row>
     <row r="12" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>1799</v>
+        <v>1652</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>1718</v>
+        <v>1794</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>1800</v>
+        <v>1795</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>1801</v>
+        <v>1796</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -23028,23 +23061,23 @@
     </row>
     <row r="13" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>1567</v>
+        <v>1654</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>1655</v>
+        <v>1797</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>1752</v>
+        <v>1798</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>1751</v>
+        <v>1799</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -23060,17 +23093,17 @@
         <v>574</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>1765</v>
+        <v>1655</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>1766</v>
+        <v>1719</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>1768</v>
+        <v>1752</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>1767</v>
+        <v>1751</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -23080,22 +23113,24 @@
     </row>
     <row r="15" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>1656</v>
+        <v>1567</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>1657</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>1745</v>
-      </c>
+        <v>1763</v>
+      </c>
+      <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>1720</v>
-      </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+        <v>1764</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>1766</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>1765</v>
+      </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
@@ -23104,17 +23139,19 @@
     </row>
     <row r="16" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>982</v>
+        <v>1656</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>1802</v>
-      </c>
-      <c r="D16" s="4"/>
+        <v>1657</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>1745</v>
+      </c>
       <c r="E16" s="4" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -23126,17 +23163,17 @@
     </row>
     <row r="17" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>1658</v>
+        <v>982</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>1803</v>
+        <v>1800</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -23148,24 +23185,20 @@
     </row>
     <row r="18" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>984</v>
+        <v>1658</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>1659</v>
+        <v>1801</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4" t="s">
-        <v>1723</v>
-      </c>
-      <c r="F18" s="65" t="s">
-        <v>1770</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>1769</v>
-      </c>
+        <v>1722</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
@@ -23174,20 +23207,24 @@
     </row>
     <row r="19" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>1660</v>
+        <v>984</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>1661</v>
+        <v>1659</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>1724</v>
-      </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+        <v>1723</v>
+      </c>
+      <c r="F19" s="65" t="s">
+        <v>1768</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>1767</v>
+      </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
@@ -23196,24 +23233,20 @@
     </row>
     <row r="20" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>1662</v>
+        <v>1660</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>1779</v>
+        <v>1661</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>1725</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>1780</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>1781</v>
-      </c>
+        <v>1724</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
@@ -23222,23 +23255,23 @@
     </row>
     <row r="21" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>1640</v>
+        <v>1662</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="C21" s="62" t="s">
-        <v>1663</v>
+      <c r="C21" s="4" t="s">
+        <v>1777</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>1757</v>
+        <v>1778</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>1786</v>
+        <v>1779</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
@@ -23248,20 +23281,24 @@
     </row>
     <row r="22" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>977</v>
+        <v>1640</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>1664</v>
+      <c r="C22" s="62" t="s">
+        <v>1663</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>1727</v>
-      </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+        <v>1726</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>1757</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>1784</v>
+      </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -23270,19 +23307,17 @@
     </row>
     <row r="23" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>1665</v>
+        <v>977</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>1666</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>1669</v>
-      </c>
+        <v>1664</v>
+      </c>
+      <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -23294,23 +23329,21 @@
     </row>
     <row r="24" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>1667</v>
+        <v>1665</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>1669</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>1804</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>1805</v>
-      </c>
+        <v>1728</v>
+      </c>
+      <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
@@ -23320,19 +23353,23 @@
     </row>
     <row r="25" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>1670</v>
+        <v>1667</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>1671</v>
-      </c>
-      <c r="D25" s="4"/>
+        <v>1668</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>1669</v>
+      </c>
       <c r="E25" s="4" t="s">
-        <v>1729</v>
-      </c>
-      <c r="F25" s="4"/>
+        <v>1802</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>1803</v>
+      </c>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
@@ -23342,19 +23379,17 @@
     </row>
     <row r="26" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>922</v>
+        <v>1670</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>1672</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>1745</v>
-      </c>
-      <c r="E26" s="38" t="s">
-        <v>1704</v>
+        <v>1671</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4" t="s">
+        <v>1729</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -23366,21 +23401,21 @@
     </row>
     <row r="27" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>1758</v>
+        <v>922</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>1759</v>
-      </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="53" t="s">
-        <v>1761</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>1760</v>
-      </c>
+        <v>1672</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>1745</v>
+      </c>
+      <c r="E27" s="38" t="s">
+        <v>1704</v>
+      </c>
+      <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
@@ -23390,25 +23425,27 @@
     </row>
     <row r="28" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>1673</v>
+        <v>1758</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>1674</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>1669</v>
-      </c>
+        <v>1759</v>
+      </c>
+      <c r="D28" s="4"/>
       <c r="E28" s="4" t="s">
-        <v>1730</v>
-      </c>
-      <c r="F28" s="4" t="s">
+        <v>2015</v>
+      </c>
+      <c r="F28" s="53" t="s">
+        <v>2013</v>
+      </c>
+      <c r="G28" s="4" t="s">
         <v>2014</v>
       </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
+      <c r="H28" s="32" t="s">
+        <v>2017</v>
+      </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -23416,20 +23453,22 @@
     </row>
     <row r="29" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>1675</v>
+        <v>1673</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>1784</v>
-      </c>
-      <c r="D29" s="4"/>
+        <v>1674</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>1669</v>
+      </c>
       <c r="E29" s="4" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>1785</v>
+        <v>2012</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
@@ -23440,19 +23479,21 @@
     </row>
     <row r="30" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>1708</v>
+        <v>1782</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4" t="s">
-        <v>1732</v>
-      </c>
-      <c r="F30" s="4"/>
+        <v>1731</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>1783</v>
+      </c>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
@@ -23462,17 +23503,17 @@
     </row>
     <row r="31" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>1678</v>
+        <v>1708</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>1734</v>
+        <v>1732</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -23490,11 +23531,11 @@
         <v>574</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -23506,17 +23547,17 @@
     </row>
     <row r="33" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>1348</v>
+        <v>1677</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
-        <v>1733</v>
+        <v>1735</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -23528,17 +23569,17 @@
     </row>
     <row r="34" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>1223</v>
+        <v>1348</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4" t="s">
-        <v>1736</v>
+        <v>1733</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
@@ -23550,17 +23591,17 @@
     </row>
     <row r="35" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>1682</v>
+        <v>1223</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>1705</v>
+        <v>1681</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
@@ -23578,18 +23619,14 @@
         <v>574</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>1683</v>
+        <v>1705</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4" t="s">
-        <v>1738</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>1763</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>1762</v>
-      </c>
+        <v>1737</v>
+      </c>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
@@ -23598,20 +23635,24 @@
     </row>
     <row r="37" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>1684</v>
+        <v>1682</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>1685</v>
+        <v>1683</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4" t="s">
-        <v>1739</v>
-      </c>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
+        <v>1738</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>1761</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>1760</v>
+      </c>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
@@ -23620,17 +23661,17 @@
     </row>
     <row r="38" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>1187</v>
+        <v>1684</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="C38" s="62" t="s">
-        <v>1686</v>
+      <c r="C38" s="4" t="s">
+        <v>1685</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -23642,17 +23683,17 @@
     </row>
     <row r="39" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>1687</v>
+        <v>1187</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>1706</v>
+      <c r="C39" s="62" t="s">
+        <v>1686</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
@@ -23664,24 +23705,20 @@
     </row>
     <row r="40" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>1771</v>
+        <v>1687</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="C40" s="15" t="s">
-        <v>1772</v>
+      <c r="C40" s="4" t="s">
+        <v>1706</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4" t="s">
-        <v>1773</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>1775</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>1774</v>
-      </c>
+        <v>1741</v>
+      </c>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
@@ -23690,23 +23727,23 @@
     </row>
     <row r="41" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>1688</v>
+        <v>1769</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>1776</v>
+      <c r="C41" s="15" t="s">
+        <v>1770</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4" t="s">
-        <v>1742</v>
+        <v>1771</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>1777</v>
+        <v>1773</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>1778</v>
+        <v>1772</v>
       </c>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
@@ -23714,62 +23751,74 @@
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
     </row>
-    <row r="42" spans="1:12" ht="87" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>986</v>
+        <v>1688</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>1707</v>
+        <v>1774</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>1753</v>
+        <v>1775</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>1754</v>
-      </c>
-      <c r="H42" s="61" t="s">
-        <v>1755</v>
-      </c>
+        <v>1776</v>
+      </c>
+      <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
     </row>
-    <row r="43" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="87" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>1689</v>
+        <v>986</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>574</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>1690</v>
+        <v>1707</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4" t="s">
-        <v>1744</v>
-      </c>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
+        <v>1743</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>1753</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>1754</v>
+      </c>
+      <c r="H43" s="61" t="s">
+        <v>1755</v>
+      </c>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
     </row>
     <row r="44" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
+      <c r="A44" s="4" t="s">
+        <v>1689</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>574</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>1690</v>
+      </c>
       <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
+      <c r="E44" s="4" t="s">
+        <v>1744</v>
+      </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
@@ -23793,18 +23842,10 @@
       <c r="L45" s="4"/>
     </row>
     <row r="46" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
-        <v>1691</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>1692</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>1669</v>
-      </c>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -23816,13 +23857,17 @@
     </row>
     <row r="47" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>1693</v>
-      </c>
-      <c r="B47" s="4"/>
+        <v>1691</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>304</v>
+      </c>
       <c r="C47" s="4" t="s">
-        <v>1694</v>
-      </c>
-      <c r="D47" s="4"/>
+        <v>1692</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>1669</v>
+      </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
@@ -23834,11 +23879,11 @@
     </row>
     <row r="48" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>1695</v>
+        <v>1693</v>
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="4" t="s">
-        <v>1696</v>
+        <v>1694</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -23852,11 +23897,11 @@
     </row>
     <row r="49" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>1697</v>
+        <v>1695</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="4" t="s">
-        <v>1698</v>
+        <v>1696</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -23870,11 +23915,11 @@
     </row>
     <row r="50" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>1699</v>
+        <v>1697</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="4" t="s">
-        <v>1700</v>
+        <v>1698</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -23888,11 +23933,11 @@
     </row>
     <row r="51" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>1689</v>
+        <v>1699</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="4" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -23905,9 +23950,13 @@
       <c r="L51" s="4"/>
     </row>
     <row r="52" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A52" s="4"/>
+      <c r="A52" s="4" t="s">
+        <v>1689</v>
+      </c>
       <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
+      <c r="C52" s="4" t="s">
+        <v>1701</v>
+      </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
@@ -23919,17 +23968,11 @@
       <c r="L52" s="4"/>
     </row>
     <row r="53" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
-        <v>1702</v>
-      </c>
+      <c r="A53" s="4"/>
       <c r="B53" s="4"/>
-      <c r="C53" s="4" t="s">
-        <v>1703</v>
-      </c>
+      <c r="C53" s="4"/>
       <c r="D53" s="4"/>
-      <c r="E53" s="4" t="s">
-        <v>1746</v>
-      </c>
+      <c r="E53" s="4"/>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
@@ -23939,11 +23982,17 @@
       <c r="L53" s="4"/>
     </row>
     <row r="54" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A54" s="4"/>
+      <c r="A54" s="4" t="s">
+        <v>1702</v>
+      </c>
       <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
+      <c r="C54" s="4" t="s">
+        <v>1703</v>
+      </c>
       <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
+      <c r="E54" s="4" t="s">
+        <v>1746</v>
+      </c>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
@@ -24064,6 +24113,20 @@
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
     </row>
+    <row r="63" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
+      <c r="K63" s="4"/>
+      <c r="L63" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
TS 1.8 Template 03/12/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9195" windowHeight="2685" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9195" windowHeight="2685" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Vowel Elongation" sheetId="1" r:id="rId1"/>
@@ -6442,13 +6442,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -6740,119 +6746,119 @@
   </cellStyleXfs>
   <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18281,7 +18287,7 @@
   <dimension ref="A2:V118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
@@ -20646,11 +20652,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V204"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C171" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="5" topLeftCell="C186" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E185" sqref="E185"/>
+      <selection pane="bottomRight" activeCell="E174" sqref="E174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22307,10 +22313,10 @@
       <c r="A141" s="29">
         <v>11.15</v>
       </c>
-      <c r="C141" s="4" t="s">
+      <c r="C141" s="32" t="s">
         <v>747</v>
       </c>
-      <c r="D141" s="4" t="s">
+      <c r="D141" s="32" t="s">
         <v>402</v>
       </c>
       <c r="G141" s="29" t="s">
@@ -22487,7 +22493,7 @@
       </c>
     </row>
     <row r="174" spans="1:5" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="E174" s="4" t="s">
+      <c r="E174" s="32" t="s">
         <v>774</v>
       </c>
     </row>
@@ -22587,7 +22593,7 @@
       </c>
     </row>
     <row r="194" spans="1:6" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="E194" s="4" t="s">
+      <c r="E194" s="32" t="s">
         <v>792</v>
       </c>
     </row>
@@ -23045,7 +23051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
GS 1.1 TS 1.6 Template etc 04/12/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9195" windowHeight="2685" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9195" windowHeight="2685" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Vowel Elongation" sheetId="1" r:id="rId1"/>
@@ -13489,7 +13489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="D36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -20652,11 +20652,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V204"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C186" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="5" topLeftCell="C129" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E174" sqref="E174"/>
+      <selection pane="bottomRight" activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
GS 4.7 and Padam temp TS 4.7 01/02/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9195" windowHeight="2685" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9195" windowHeight="2685" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Vowel Elongation" sheetId="1" r:id="rId1"/>
@@ -7155,7 +7155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L192"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
+    <sheetView topLeftCell="A97" workbookViewId="0">
       <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
@@ -13504,7 +13504,7 @@
   <dimension ref="A2:X114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="G37" sqref="G37"/>
@@ -18300,8 +18300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V118"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="5" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="D110" sqref="D110"/>
@@ -20666,11 +20666,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C150" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="5" topLeftCell="C186" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E179" sqref="E179"/>
+      <selection pane="bottomRight" activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21624,7 +21624,7 @@
       </c>
     </row>
     <row r="90" spans="1:22" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="E90" s="4" t="s">
+      <c r="E90" s="32" t="s">
         <v>708</v>
       </c>
       <c r="G90" s="29" t="s">

</xml_diff>

<commit_message>
Chamaka, TB etc 16/02/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5F3515-CA84-44C3-A022-2FA1538ACFF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9195" windowHeight="2685" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vowel Elongation" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
     <sheet name="Special Anuswaram" sheetId="8" r:id="rId8"/>
     <sheet name="Special Test Cases" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -6441,7 +6442,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -7152,7 +7153,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L192"/>
   <sheetViews>
     <sheetView topLeftCell="A97" workbookViewId="0">
@@ -10563,7 +10564,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:N218"/>
   <sheetViews>
     <sheetView topLeftCell="B2" workbookViewId="0">
@@ -12679,7 +12680,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:Q46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13500,7 +13501,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:X114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15550,10 +15551,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A3:U294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+    <sheetView topLeftCell="A130" workbookViewId="0">
       <selection activeCell="L127" sqref="L127"/>
     </sheetView>
   </sheetViews>
@@ -18297,7 +18298,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:V118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20663,14 +20664,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A2:V204"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C186" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="5" topLeftCell="C78" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E90" sqref="E90"/>
+      <selection pane="bottomRight" activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22664,7 +22665,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A2:G113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23080,7 +23081,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A2:L63"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">

</xml_diff>

<commit_message>
Padam files Jatai 20/02/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5F3515-CA84-44C3-A022-2FA1538ACFF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8D77EF-99B2-44BC-B0B5-B9054F8184DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20668,10 +20668,10 @@
   <dimension ref="A2:V204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C78" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E93" sqref="E93"/>
+      <selection pane="bottomRight" activeCell="I76" sqref="I76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TS 4.5 Ghanam with JM/JD ref 23/07/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8659026-F31C-423A-B9E1-C67513B537D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80B3494-0022-486A-ABAC-C3CCFEF99086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vowel Elongation" sheetId="1" r:id="rId1"/>
@@ -6769,7 +6769,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6888,6 +6888,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13519,7 +13520,7 @@
   <dimension ref="A2:X114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="G37" sqref="G37"/>
@@ -15568,7 +15569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A3:U294"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A127" workbookViewId="0">
       <selection activeCell="L127" sqref="L127"/>
     </sheetView>
   </sheetViews>
@@ -23098,8 +23099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A2:L63"/>
   <sheetViews>
-    <sheetView topLeftCell="D13" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23197,7 +23198,7 @@
       <c r="F5" s="4" t="s">
         <v>1766</v>
       </c>
-      <c r="G5" s="80" t="s">
+      <c r="G5" s="82" t="s">
         <v>1767</v>
       </c>
       <c r="H5" s="4"/>

</xml_diff>

<commit_message>
TS 1.6 Ghanam Jatai input files 18/01/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D82FFD-10AA-4263-80B8-BD5DBA9F941A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B88B379-5FDD-405B-8063-796E470EDBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vowel Elongation" sheetId="1" r:id="rId1"/>
@@ -12711,7 +12711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:Q46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -23112,7 +23112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A2:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
nmv 15 02 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\texts\TS Jatai Working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B88B379-5FDD-405B-8063-796E470EDBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Vowel Elongation" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
     <sheet name="Special Anuswaram" sheetId="8" r:id="rId8"/>
     <sheet name="Special Test Cases" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3457" uniqueCount="2074">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3458" uniqueCount="2075">
   <si>
     <t xml:space="preserve">PrAtiSakyam Rules </t>
   </si>
@@ -6445,11 +6444,14 @@
   <si>
     <t>acCA</t>
   </si>
+  <si>
+    <t>2.2.4.8(11)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -7181,7 +7183,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L192"/>
   <sheetViews>
     <sheetView topLeftCell="A100" workbookViewId="0">
@@ -10592,7 +10594,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N218"/>
   <sheetViews>
     <sheetView topLeftCell="B151" workbookViewId="0">
@@ -12708,10 +12710,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -13529,7 +13531,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15579,7 +15581,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:U294"/>
   <sheetViews>
     <sheetView topLeftCell="A127" workbookViewId="0">
@@ -18326,7 +18328,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20692,14 +20694,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V204"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C42" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="5" topLeftCell="C151" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="I76" sqref="I76"/>
+      <selection pane="bottomRight" activeCell="I155" sqref="I155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20708,6 +20710,7 @@
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
@@ -22410,82 +22413,85 @@
         <v>748</v>
       </c>
     </row>
-    <row r="145" spans="4:4" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="145" spans="4:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D145" s="4" t="s">
         <v>768</v>
       </c>
     </row>
-    <row r="146" spans="4:4" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="146" spans="4:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D146" s="4" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="147" spans="4:4" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="147" spans="4:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D147" s="4" t="s">
         <v>750</v>
       </c>
     </row>
-    <row r="148" spans="4:4" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="148" spans="4:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D148" s="4" t="s">
         <v>751</v>
       </c>
     </row>
-    <row r="149" spans="4:4" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="149" spans="4:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D149" s="4" t="s">
         <v>752</v>
       </c>
     </row>
-    <row r="150" spans="4:4" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="150" spans="4:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D150" s="4" t="s">
         <v>753</v>
       </c>
     </row>
-    <row r="151" spans="4:4" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="151" spans="4:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D151" s="4" t="s">
         <v>754</v>
       </c>
     </row>
-    <row r="152" spans="4:4" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="152" spans="4:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D152" s="4" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="153" spans="4:4" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="153" spans="4:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D153" s="4" t="s">
         <v>756</v>
       </c>
     </row>
-    <row r="154" spans="4:4" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="154" spans="4:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D154" s="4" t="s">
         <v>860</v>
       </c>
     </row>
-    <row r="155" spans="4:4" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="D155" s="4" t="s">
+    <row r="155" spans="4:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="D155" s="32" t="s">
         <v>757</v>
       </c>
-    </row>
-    <row r="156" spans="4:4" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="I155" s="29" t="s">
+        <v>2074</v>
+      </c>
+    </row>
+    <row r="156" spans="4:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D156" s="4" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="157" spans="4:4" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="157" spans="4:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D157" s="4" t="s">
         <v>759</v>
       </c>
     </row>
-    <row r="158" spans="4:4" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="158" spans="4:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D158" s="32" t="s">
         <v>1078</v>
       </c>
     </row>
-    <row r="159" spans="4:4" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="159" spans="4:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D159" s="4" t="s">
         <v>760</v>
       </c>
     </row>
-    <row r="160" spans="4:4" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="160" spans="4:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D160" s="4" t="s">
         <v>761</v>
       </c>
@@ -22693,7 +22699,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23109,7 +23115,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L63"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">

</xml_diff>

<commit_message>
TS 3.1 Padam Hearing - 05/04/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E62CFCB-861E-45C8-A8EA-193490B78CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0732ADD1-0E62-4101-9ED3-A2E5CE07D644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6454,13 +6454,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -6788,125 +6794,125 @@
   </cellStyleXfs>
   <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -20703,7 +20709,7 @@
   <dimension ref="A2:V204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C111" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="E56" sqref="E56"/>

</xml_diff>

<commit_message>
Excel Templates 2.5,2.6 and 3.2
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCF7DC2-A50C-48FB-9BCF-71BEB0BEAE96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A650BFA8-D2B3-4390-9AE1-40D636F2CCDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vowel Elongation" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3459" uniqueCount="2076">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3460" uniqueCount="2077">
   <si>
     <t xml:space="preserve">PrAtiSakyam Rules </t>
   </si>
@@ -6451,6 +6451,9 @@
   </si>
   <si>
     <t>3.2.5.7</t>
+  </si>
+  <si>
+    <t>2.5.8.6</t>
   </si>
 </sst>
 </file>
@@ -12734,7 +12737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -20718,11 +20721,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A2:V204"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E192" sqref="E192"/>
+      <selection pane="bottomRight" activeCell="I164" sqref="I164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22517,57 +22520,60 @@
         <v>760</v>
       </c>
     </row>
-    <row r="161" spans="1:5" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D161" s="4" t="s">
         <v>761</v>
       </c>
     </row>
-    <row r="162" spans="1:5" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D162" s="32" t="s">
         <v>768</v>
       </c>
     </row>
-    <row r="163" spans="1:5" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D163" s="32" t="s">
         <v>762</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="I163" s="29" t="s">
+        <v>2076</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D164" s="32" t="s">
         <v>763</v>
       </c>
     </row>
-    <row r="165" spans="1:5" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D165" s="4" t="s">
         <v>843</v>
       </c>
     </row>
-    <row r="166" spans="1:5" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D166" s="32" t="s">
         <v>769</v>
       </c>
     </row>
-    <row r="167" spans="1:5" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D167" s="32" t="s">
         <v>764</v>
       </c>
     </row>
-    <row r="168" spans="1:5" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D168" s="69" t="s">
         <v>2058</v>
       </c>
     </row>
-    <row r="169" spans="1:5" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="D169" s="4" t="s">
         <v>765</v>
       </c>
     </row>
-    <row r="170" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="D170" s="32" t="s">
         <v>766</v>
       </c>
     </row>
-    <row r="172" spans="1:5" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A172" s="4">
         <v>11.17</v>
       </c>
@@ -22575,22 +22581,22 @@
         <v>770</v>
       </c>
     </row>
-    <row r="173" spans="1:5" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="E173" s="4" t="s">
         <v>771</v>
       </c>
     </row>
-    <row r="174" spans="1:5" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="E174" s="32" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="175" spans="1:5" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="E175" s="4" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="176" spans="1:5" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="E176" s="4" t="s">
         <v>774</v>
       </c>

</xml_diff>

<commit_message>
TS 2.5 Files, Articles as edited - 30/06/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224C1EC3-62DF-4CCA-88A7-D81461260EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BF5357-69A3-4C1E-9256-489466030A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20722,7 +20722,7 @@
   <dimension ref="A2:V204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C117" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C105" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="D119" sqref="D119"/>

</xml_diff>

<commit_message>
TS 4.7 Tamil Ghanam Jatai final - 23/03/2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
+++ b/TS Jatai Working/prAtiSAkyam Rules Sethu.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3852464E-918E-4680-B4DF-003B80195198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CC9F8D-2ACE-4162-9A40-D62F2C82253C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6460,13 +6460,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -6806,124 +6812,124 @@
   </cellStyleXfs>
   <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="24" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="36" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -20699,10 +20705,10 @@
   <dimension ref="A2:V204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C168" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D169" sqref="D169"/>
+      <selection pane="bottomRight" activeCell="E190" sqref="E190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>